<commit_message>
Tue Nov 28 06:50:04 AM CST 2023
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1057,7 +1058,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1103,7 +1104,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1129,7 +1130,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1149,7 +1150,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1175,7 +1176,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1195,7 +1196,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>45125</v>
       </c>
       <c r="B4">
@@ -1221,7 +1222,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1241,7 +1242,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1267,7 +1268,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="6">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1287,7 +1288,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1313,7 +1314,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1333,7 +1334,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1359,7 +1360,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1379,7 +1380,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1405,7 +1406,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1425,7 +1426,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1451,7 +1452,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="6">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1471,7 +1472,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1497,7 +1498,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="6">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1517,7 +1518,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5">
+      <c r="A11" s="6">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1543,7 +1544,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="6">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1563,7 +1564,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5">
+      <c r="A12" s="6">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1589,7 +1590,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="6">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1609,7 +1610,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5">
+      <c r="A13" s="6">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1635,7 +1636,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="6">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1655,7 +1656,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5">
+      <c r="A14" s="6">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1681,7 +1682,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="6">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1701,7 +1702,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1727,7 +1728,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="6">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1747,7 +1748,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5">
+      <c r="A16" s="6">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1773,7 +1774,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="6">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1793,7 +1794,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5">
+      <c r="A17" s="6">
         <v>45247</v>
       </c>
       <c r="B17">
@@ -1819,7 +1820,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="6">
         <v>45245</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1839,7 +1840,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5">
+      <c r="A18" s="6">
         <v>45252</v>
       </c>
       <c r="B18">
@@ -1865,7 +1866,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="6">
         <v>45246</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1879,6 +1880,52 @@
         </is>
       </c>
       <c r="J18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6">
+        <v>45257</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>曹卓补充订单</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G19" s="6">
+        <v>45253</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>待完成</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>曹卓交付三个订单所需数据</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1941,7 +1988,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -1967,7 +2014,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1987,7 +2034,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -2013,7 +2060,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -2033,7 +2080,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -2059,7 +2106,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Thu Nov 30 06:50:04 AM CST 2023
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,8 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
@@ -1058,7 +1060,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1104,7 +1106,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="6">
+      <c r="A2" s="8">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1130,7 +1132,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="8">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1150,7 +1152,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="8">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1176,7 +1178,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="8">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1196,7 +1198,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="8">
         <v>45125</v>
       </c>
       <c r="B4">
@@ -1222,7 +1224,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="8">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1242,7 +1244,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="8">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1268,7 +1270,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="8">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1288,7 +1290,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="8">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1314,7 +1316,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="8">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1334,7 +1336,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="8">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1360,7 +1362,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="8">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1380,7 +1382,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1406,7 +1408,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="8">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1426,7 +1428,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="8">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1452,7 +1454,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="8">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1472,7 +1474,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6">
+      <c r="A10" s="8">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1498,7 +1500,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="8">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1518,7 +1520,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6">
+      <c r="A11" s="8">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1544,7 +1546,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="8">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1564,7 +1566,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6">
+      <c r="A12" s="8">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1590,7 +1592,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="8">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1610,7 +1612,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6">
+      <c r="A13" s="8">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1636,7 +1638,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="8">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1656,7 +1658,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6">
+      <c r="A14" s="8">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1682,7 +1684,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="8">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1702,7 +1704,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6">
+      <c r="A15" s="8">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1728,7 +1730,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="8">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1748,7 +1750,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6">
+      <c r="A16" s="8">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1774,7 +1776,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="8">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1794,25 +1796,25 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="6">
-        <v>45247</v>
+      <c r="A17" s="8">
+        <v>45258</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 01-订单编号：IN2023110603 02-区域-销售：杭州-吴航贵 03-上级主管：王立家 04-医院：浙江大学医学院附属儿童医院 05-科室/职称：眼科/主治 06-电话： 07-项目（确定A/B套餐）：润色代发sci3-4分，客户自己文章 08-分值：3-4分 09-定题题目：octa技术在糖尿病视网膜病变中的应用 10-时间要求：45天 11-总价： 12-定金：已付 13-评估人员 ： 14-技术支持（沟通情况）：薛富才（沟通次数）2次， 15-附件：客户资料 16-备注： 16.1客户要求：cover letter 也帮客户拟掉，后面老板和编辑部有修改意见也帮忙修改下  17-项目负责人：杨啸 </t>
+          <t/>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>IN2023110603</t>
+          <t>曹卓肺癌和癌旁组织对比分析</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t/>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1820,8 +1822,8 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="6">
-        <v>45245</v>
+      <c r="G17" s="8">
+        <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1830,7 +1832,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>OCTA 在糖尿病视网膜病变中的应用</t>
+          <t>肺癌和癌旁组织单细胞数据对比分析</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1840,25 +1842,25 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6">
-        <v>45252</v>
+      <c r="A18" s="8">
+        <v>45247</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t/>
+          <t xml:space="preserve"> 01-订单编号：IN2023110603 02-区域-销售：杭州-吴航贵 03-上级主管：王立家 04-医院：浙江大学医学院附属儿童医院 05-科室/职称：眼科/主治 06-电话： 07-项目（确定A/B套餐）：润色代发sci3-4分，客户自己文章 08-分值：3-4分 09-定题题目：octa技术在糖尿病视网膜病变中的应用 10-时间要求：45天 11-总价： 12-定金：已付 13-评估人员 ： 14-技术支持（沟通情况）：薛富才（沟通次数）2次， 15-附件：客户资料 16-备注： 16.1客户要求：cover letter 也帮客户拟掉，后面老板和编辑部有修改意见也帮忙修改下  17-项目负责人：杨啸 </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>A2023060507</t>
+          <t>IN2023110603</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1866,8 +1868,8 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="6">
-        <v>45246</v>
+      <c r="G18" s="8">
+        <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1876,7 +1878,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>脓毒症肠损伤联合肠道菌与代谢物分析</t>
+          <t>OCTA 在糖尿病视网膜病变中的应用</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1886,8 +1888,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6">
-        <v>45257</v>
+      <c r="A19" s="8">
+        <v>45252</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1899,33 +1901,79 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>A2023060507</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G19" s="8">
+        <v>45246</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>脓毒症肠损伤联合肠道菌与代谢物分析</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8">
+        <v>45257</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>曹卓补充订单</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
         <is>
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="6">
+      <c r="G20" s="8">
         <v>45253</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>待完成</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>曹卓交付三个订单所需数据</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1988,7 +2036,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="6">
+      <c r="A2" s="8">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -2014,7 +2062,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="8">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -2034,7 +2082,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="8">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -2060,7 +2108,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="8">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -2080,7 +2128,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="8">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -2106,7 +2154,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="8">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Thu Dec 28 06:50:04 AM CST 2023
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -1060,7 +1061,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1106,7 +1107,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1132,7 +1133,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1152,7 +1153,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1178,7 +1179,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1198,8 +1199,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8">
-        <v>45125</v>
+      <c r="A4" s="9">
+        <v>45156</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1216,7 +1217,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t/>
+          <t>/</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1224,7 +1225,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1244,7 +1245,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1270,7 +1271,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1290,7 +1291,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1316,7 +1317,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="9">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1336,7 +1337,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8">
+      <c r="A7" s="9">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1362,7 +1363,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="9">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1382,7 +1383,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8">
+      <c r="A8" s="9">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1408,7 +1409,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="9">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1428,7 +1429,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8">
+      <c r="A9" s="9">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1454,7 +1455,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="9">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1474,7 +1475,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8">
+      <c r="A10" s="9">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1500,7 +1501,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="9">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1520,7 +1521,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1546,7 +1547,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="9">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1566,7 +1567,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8">
+      <c r="A12" s="9">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1592,7 +1593,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="9">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1612,7 +1613,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8">
+      <c r="A13" s="9">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1638,7 +1639,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="9">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1658,7 +1659,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1684,7 +1685,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="9">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1704,7 +1705,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8">
+      <c r="A15" s="9">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1730,7 +1731,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="9">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1750,7 +1751,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8">
+      <c r="A16" s="9">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1776,7 +1777,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="9">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1796,7 +1797,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8">
+      <c r="A17" s="9">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1822,7 +1823,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="9">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1842,7 +1843,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="8">
+      <c r="A18" s="9">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1868,7 +1869,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="9">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1888,7 +1889,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8">
+      <c r="A19" s="9">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1914,7 +1915,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="9">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1934,7 +1935,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="8">
+      <c r="A20" s="9">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1960,7 +1961,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="9">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1974,6 +1975,558 @@
         </is>
       </c>
       <c r="J20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9">
+        <v>45264</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2021112501-原始数据提供</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G21" s="9">
+        <v>45260</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>原始数据提供</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9">
+        <v>45265</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Treg 细胞差异表达基因</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G22" s="9">
+        <v>45264</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>ccRCC 单细胞数据的 Treg 细胞差异表达基因</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9">
+        <v>45272</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：IN2023120404 02-区域-销售：付梓欣 03-上级主管：王立家 04-医院：浙江省人民医院 05-科室/职称：康复科 06-电话： 07-项目（确定A/B套餐）：生信分析 08-分值：sci 1.5-2(生信) 09-定题题目：无 10-时间要求：2025年5月31前 11-总价： 12-定金：已付 13-评估人员 ：陶安琪，孙慧 14-技术支持（沟通情况）：薛富才（1次）。客户做生信，与客户课题相关。15-附件：评估邮件汇总，临床实验方案 16-备注：16-1.客户分级（需要文章晋升，或者单纯课题结题。老客户。） 16-2.谈单承诺,（与客户课题具有相关性；不投中科院预警杂志。） 17-项目负责人：杨弘 客户：章玮 </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>IN2023120404</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1.5-2</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G23" s="9">
+        <v>45264</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>RNA-seq 探究 rTMS 对 SCI 和 NP 的影响</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9">
+        <v>45266</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：实验：S2023120402；毕业论文：N2023120403 02-区域-销售：吴晓凤、叶立欢 03-上级主管： 04-医院：富阳第一人民医院 05-科室/职称： 06-电话： 07-项目（确定A/B套餐）：实验+毕业论文 08-分值： 09-定题题目： 10-时间要求：2024年3月 11-总价： 12-定金：已付 13-评估人员 ：陈颖+吴晓凤 14-技术支持（沟通情况）：吴晓凤 15-附件：定金，报价，技术支持与客户沟通总结 16-备注：1.客户实验+毕业论文） 2.谈单承诺,（复方细胞实验只提供三次有效数据，动物实验的材料由我司代买，客户自己付钱，动物检测部分结束后会给蜡块及切片） 17-项目负责人：杨弘 </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>实验：S2023120402；毕业论文：N2023120403</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G24" s="9">
+        <v>45266</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>补肾健脾汤网络药理学分析</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9">
+        <v>45266</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>半夏泻心汤网络药理学分析</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G25" s="9">
+        <v>45266</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>半夏泻心汤网络药理学分析</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9">
+        <v>45268</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>方和敬-白茅根-IgA网络药理学分析</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G26" s="9">
+        <v>45267</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>白茅根-IgA网络药理学分析</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9">
+        <v>45275</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>S2023110704</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G27" s="9">
+        <v>45272</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>RNA的结合位点</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9">
+        <v>45273</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>陈云杰测序结果差异分析</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G28" s="9">
+        <v>45272</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>测序结果差异分析</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9">
+        <v>45274</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SN2023011001</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G29" s="9">
+        <v>45274</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>陈云杰测序数据分析++</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="9">
+        <v>45274</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号： 02-区域-销售：江苏-郭树仁 03-上级主管：王立家 04-医院：浙江省中 05-科室/职称：耳鼻喉科 06-电话： 07-项目（确定A/B套餐）：A 08-分值：3-5分 中科院三区 09-定题题目： 10-时间要求：2023/11/23-2025/5/23（18月）1月15日给国青标书，24年6月份给中管局、卫生厅标书， 11-总价： 12-定金： 13-评估人员 ：吴晨 14-技术支持（沟通情况）：薛富才（4次），吴晨 15-附件：定金截图（包含标书），方案，合同，实验报价 16-备注：1.潜力客户，做项目为了后续拿课题。 2.谈单承诺,（沟通过程中有答应客户的要求请尽数附上）：1月中给国青标书，6月初给中管局、卫生厅标书，先做预实验，争取国青本子中包含一点数据结果（和吴晓凤经理沟通过） 3、实验分阶段进行，除了与课题相关的实验部分，后续文章部分的实验等通知再进行。此外预实验分成两大模块，具体情况可与售前技术吴晨或者薛富才沟通。 4、所有实验需要走实验项目，需要实验分阶段汇报，动物实验保存图片和视频。 </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>A2023112405</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>sci3-5分 中科院三区</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G30" s="9">
+        <v>45274</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>靳阳子生信支持业务</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="9">
+        <v>45285</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：IN2023122103 02-区域-销售：周燕青 03-上级主管：柳叶 04-医院： 05-科室/职称：消化内科 06-电话： 07-项目（确定A/B套餐）：生信分析 08-分值： 09-定题题目： 10-时间要求：2023年12月27日前完成 11-总价： 12-定金：已付（结清） 13-评估人员 ：林婧羽  14-技术支持：林婧羽、薛富才（沟通情况）： 15-附件：后续合同再补充  </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>IN2023122103</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G31" s="9">
+        <v>45281</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>胆结石RNA-seq结合肠道菌、代谢物筛选关键差异表达基因</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="9">
+        <v>45285</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>周芳药方-草药-单体-靶点</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G32" s="9">
+        <v>45281</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>X药方-草药-单体-靶点</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2036,7 +2589,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -2062,7 +2615,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -2082,7 +2635,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -2108,7 +2661,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -2128,7 +2681,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -2154,7 +2707,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Fri Feb  2 06:50:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -1061,7 +1062,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1107,7 +1108,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="9">
+      <c r="A2" s="10">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1133,7 +1134,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="10">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1153,7 +1154,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9">
+      <c r="A3" s="10">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1179,7 +1180,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="10">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1199,7 +1200,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9">
+      <c r="A4" s="10">
         <v>45156</v>
       </c>
       <c r="B4">
@@ -1225,7 +1226,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="10">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1245,7 +1246,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9">
+      <c r="A5" s="10">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1271,7 +1272,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="10">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1291,7 +1292,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9">
+      <c r="A6" s="10">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1317,7 +1318,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="10">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1337,7 +1338,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9">
+      <c r="A7" s="10">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1363,7 +1364,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="10">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1383,7 +1384,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9">
+      <c r="A8" s="10">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1409,7 +1410,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="10">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1429,7 +1430,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9">
+      <c r="A9" s="10">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1455,7 +1456,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="10">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1475,7 +1476,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9">
+      <c r="A10" s="10">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1501,7 +1502,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="10">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1521,7 +1522,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9">
+      <c r="A11" s="10">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1547,7 +1548,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="10">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1567,7 +1568,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9">
+      <c r="A12" s="10">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1593,7 +1594,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="10">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1613,7 +1614,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9">
+      <c r="A13" s="10">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1639,7 +1640,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="10">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1659,7 +1660,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9">
+      <c r="A14" s="10">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1685,7 +1686,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="10">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1705,7 +1706,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9">
+      <c r="A15" s="10">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1731,7 +1732,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="10">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1751,7 +1752,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9">
+      <c r="A16" s="10">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1777,7 +1778,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="10">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1797,7 +1798,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9">
+      <c r="A17" s="10">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1823,7 +1824,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="10">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1843,7 +1844,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9">
+      <c r="A18" s="10">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1869,7 +1870,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="10">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1889,7 +1890,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="9">
+      <c r="A19" s="10">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1915,7 +1916,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="10">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1935,7 +1936,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9">
+      <c r="A20" s="10">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1961,7 +1962,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="10">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1981,7 +1982,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9">
+      <c r="A21" s="10">
         <v>45264</v>
       </c>
       <c r="B21">
@@ -2007,7 +2008,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="10">
         <v>45260</v>
       </c>
       <c r="H21" t="inlineStr">
@@ -2027,7 +2028,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="9">
+      <c r="A22" s="10">
         <v>45265</v>
       </c>
       <c r="B22">
@@ -2053,7 +2054,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="10">
         <v>45264</v>
       </c>
       <c r="H22" t="inlineStr">
@@ -2073,7 +2074,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="9">
+      <c r="A23" s="10">
         <v>45272</v>
       </c>
       <c r="B23">
@@ -2099,7 +2100,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="10">
         <v>45264</v>
       </c>
       <c r="H23" t="inlineStr">
@@ -2119,7 +2120,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="9">
+      <c r="A24" s="10">
         <v>45266</v>
       </c>
       <c r="B24">
@@ -2145,7 +2146,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="10">
         <v>45266</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -2165,7 +2166,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="9">
+      <c r="A25" s="10">
         <v>45266</v>
       </c>
       <c r="B25">
@@ -2191,7 +2192,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="10">
         <v>45266</v>
       </c>
       <c r="H25" t="inlineStr">
@@ -2211,7 +2212,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="9">
+      <c r="A26" s="10">
         <v>45268</v>
       </c>
       <c r="B26">
@@ -2237,7 +2238,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="10">
         <v>45267</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -2257,7 +2258,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="9">
+      <c r="A27" s="10">
         <v>45275</v>
       </c>
       <c r="B27">
@@ -2283,7 +2284,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="10">
         <v>45272</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -2303,7 +2304,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="9">
+      <c r="A28" s="10">
         <v>45273</v>
       </c>
       <c r="B28">
@@ -2329,7 +2330,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="10">
         <v>45272</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -2349,7 +2350,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9">
+      <c r="A29" s="10">
         <v>45274</v>
       </c>
       <c r="B29">
@@ -2375,7 +2376,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="10">
         <v>45274</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -2395,8 +2396,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="9">
-        <v>45274</v>
+      <c r="A30" s="10">
+        <v>45295</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -2421,7 +2422,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="10">
         <v>45274</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -2431,7 +2432,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>靳阳子生信支持业务</t>
+          <t>白芍网络药理学</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2441,8 +2442,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="9">
-        <v>45285</v>
+      <c r="A31" s="10">
+        <v>45293</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -2467,7 +2468,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="10">
         <v>45281</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -2487,7 +2488,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="9">
+      <c r="A32" s="10">
         <v>45285</v>
       </c>
       <c r="B32">
@@ -2513,7 +2514,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="10">
         <v>45281</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -2527,6 +2528,374 @@
         </is>
       </c>
       <c r="J32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10">
+        <v>45306</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>N2023121508</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G33" s="10">
+        <v>45288</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>网络药理学分析+蛋白对接模拟</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="10">
+        <v>45303</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>黎文华菌群+对应代谢产物介导+机制研究</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G34" s="10">
+        <v>45299</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>菌群+对应代谢产物介导+机制研究</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="10">
+        <v>45322</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>张郜晨茜红豆杉和养阴解毒汤的共同活性成分和作用靶点（m6A、铁死亡相关)</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G35" s="10">
+        <v>45299</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>红豆杉和养阴解毒汤的共同活性成分和作用靶点（m6A、铁死亡相关)</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="10">
+        <v>45323</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：A2023112804（实验走实验项目） 02-区域-销售：江苏 郭树仁 03-上级主管：王立家 04-医院：中山医院 05-科室/职称：内分泌 主治 06-电话： 07-项目（确定A/B套餐）：A 08-分值：sci3-5 09-定题题目： 10-时间要求：2023/11/23-2025/5/23（18月） 11-总价： 12-定金：已付 13-评估人员 ：吴萌硕 14-技术支持（沟通情况）：薛富才（2）吴萌硕。 15-附件：定金截图、合同、报价单、技术路线图 16-备注： 16-1潜力客户，做项目为了后续拿课题。王总对接过来的 16-2谈单承诺：实验中的嘌呤先用国产如果效果不好用进口，价格是抹去的。等省自然结果出来后，如果中标，修改方案结题，如果不中，再次签订标书合同。 16-3实验分阶段进行，需要实验汇报，实验过程需要保留视频和图片（动物实验层面） 16-4所有实验需要走实验项目 17-项目负责人：杨弘 内部要求：  1）内部留存原始数据，三次重复实验 2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通；   </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>A2023112804</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>sci3-5</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G36" s="10">
+        <v>45302</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>质谱+网络药理学分析</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="10">
+        <v>45322</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>周宇查询学者发文和 H 指数</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G37" s="10">
+        <v>45303</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>查询学者发文和 H 指数</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="10">
+        <v>45322</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>雅威1月业务审核</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G38" s="10">
+        <v>45314</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>雅威1月业务审核</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="10">
+        <v>45321</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：IN2024012502  02-区域-销售：周燕青 03-上级主管：柳叶 04-医院：上海第六人民医院 05-科室/职称：消化内科 06-电话： 07-项目（确定A/B套餐）：生信分析 08-分值：/ 09-定题题目： 10-时间要求：2024年2月2日完成 11-总价： 12-定金：已付 13-评估人员 ：林婧宇  14-技术支持：林婧宇、薛富才（沟通情况）： 15-附件：1、后续合同再补充  2、技术支持与客户沟通反馈总结 3、优惠价领导审批 16-备注： 客户要求： 1）客户分级：潜力客户，做项目为了后续拿课题。 2）谈单承诺：新增肠道菌群的宏基因组分析，客户希望结合RNAseq一起做，别到时候分析好发现还有其他的需要再次分析的，考虑周全。已申请优惠，请参考附件图。 内部要求： 加急 17-项目负责人：杨弘 </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>IN2024012502</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G39" s="10">
+        <v>45317</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>肠道菌群宏基因组群落分析联合RNA-seq</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="10">
+        <v>45322</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>N2023121805</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>无</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G40" s="10">
+        <v>45300</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>网络药理学+Mandenol与piezo1分子对接</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2589,7 +2958,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="9">
+      <c r="A2" s="10">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -2615,7 +2984,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="10">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -2635,7 +3004,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9">
+      <c r="A3" s="10">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -2661,7 +3030,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="10">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -2681,7 +3050,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9">
+      <c r="A4" s="10">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -2707,7 +3076,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="10">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Sat Feb  3 06:50:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -1108,7 +1109,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="10">
+      <c r="A2" s="11">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1134,7 +1135,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="11">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1149,12 +1150,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 挖掘 HERB 数据库; (3) 获取疾病或条件相关的基因集:Genecards; (4) 构建 PPI 网络; (5) KEGG、GO富集分析</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1180,7 +1181,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="11">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1195,12 +1196,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 全自动批量分子对接</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>45156</v>
       </c>
       <c r="B4">
@@ -1226,7 +1227,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="11">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1241,12 +1242,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从头开始的 RNA-seq 数据分析:从fastq开始质控、注释等; (2) RNA-seq 差异分析; (3) 基因注释、信息获取; (4) WGCNA 共表达分析; (5) RBP 预测:RNA 结合蛋白与 RNA 的结合</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1272,7 +1273,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="11">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1287,12 +1288,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 挖掘 HERB 数据库; (2) 网络药理学; (3) 获取疾病或条件相关的基因集:Genecards; (4) 构建 PPI 网络; (5) KEGG、GO富集分析; (6) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等; (7) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (8) 从公共数据库挖掘可用的 16s RNA 肠道菌群数据; (9) 从公共数据库挖掘可用的代谢物数据; (10) 全自动批量分子对接; (11) 代谢物富集分析</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10">
+      <c r="A6" s="11">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1318,7 +1319,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="11">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1333,12 +1334,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从头开始的WES数据分析:从fastq开始质控、注释等; (2) WES 变异筛选; (3) KEGG、GO富集分析</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10">
+      <c r="A7" s="11">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1364,7 +1365,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="11">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1379,12 +1380,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 挖掘 HERB 数据库; (2) 网络药理学; (3) 获取疾病或条件相关的基因集:Genecards; (4) 构建 PPI 网络; (5) KEGG、GO富集分析; (6) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等; (7) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (8) 从公共数据库挖掘可用的 16s RNA 肠道菌群数据; (9) 从公共数据库挖掘可用的代谢物数据; (10) 全自动批量分子对接; (11) 代谢物富集分析</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10">
+      <c r="A8" s="11">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1410,7 +1411,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="11">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1425,12 +1426,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从 GEO 挖掘可用数据:RNA-seq; (2) TCGA 数据挖掘和常规分析; (3) RNA-seq 差异分析; (4) KEGG、GO富集分析; (5) Pathview 可视化富集通路; (6) WGCNA 共表达分析</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10">
+      <c r="A9" s="11">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1456,7 +1457,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="11">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1471,12 +1472,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 制作特定功能的 R 包; (2) 蛋白质 pdb 数据获取用于可视化; (3) 蛋白质信息获取</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10">
+      <c r="A10" s="11">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1502,7 +1503,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="11">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1517,12 +1518,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从头开始的 RNA-seq 数据分析:从fastq开始质控、注释等; (2) 差异分析; (3) 富集分析; (4) 从 GEO 挖掘可用数据:RNA-seq; (5) 全自动批量分子对接; (6) 从公共数据库挖掘可用的代谢物数据; (7) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (8) 代谢物富集分析; (9) 蛋白质或基因和代谢物数据联合分析:通过公共数据挖掘建立联系; (10) 铁死亡相关基因挖掘; (11) GSEA 富集分析</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10">
+      <c r="A11" s="11">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1548,7 +1549,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="11">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1563,12 +1564,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从头开始的 RNA-seq 数据分析:从fastq开始质控、注释等; (2) 差异分析; (3) 富集分析; (4) 从 GEO 挖掘可用数据:RNA-seq; (5) 全自动批量分子对接; (6) 从公共数据库挖掘可用的代谢物数据; (7) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (8) 代谢物富集分析; (9) 蛋白质或基因和代谢物数据联合分析:通过公共数据挖掘建立联系; (10) 铁死亡相关基因挖掘; (11) GSEA 富集分析</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1594,7 +1595,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="11">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1609,12 +1610,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从头开始的 RNA-seq 数据分析:从fastq开始质控、注释等; (2) 差异分析; (3) 富集分析; (4) 从 GEO 挖掘可用数据:RNA-seq; (5) 全自动批量分子对接; (6) 从公共数据库挖掘可用的代谢物数据; (7) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (8) 代谢物富集分析; (9) 蛋白质或基因和代谢物数据联合分析:通过公共数据挖掘建立联系; (10) 铁死亡相关基因挖掘; (11) GSEA 富集分析</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10">
+      <c r="A13" s="11">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1640,7 +1641,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="11">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1655,12 +1656,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 空间转录组常规分析:大致同单细胞数据; (2) 细胞注释; (3) 拟时分析; (4) 单细胞细胞通讯; (5) 单细胞数据鉴定癌细胞; (6) 以拟时分析区分细胞亚群</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10">
+      <c r="A14" s="11">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1686,7 +1687,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="11">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1701,12 +1702,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从 GEO 挖掘可用数据:RNA-seq; (2) 挖掘 HERB 数据库; (3) 构建 PPI 网络; (4) Pathview 可视化富集通路; (5) KEGG、GO富集分析</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10">
+      <c r="A15" s="11">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1732,7 +1733,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="11">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1747,12 +1748,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) RBP 预测:RNA 结合蛋白与 RNA 的结合; (2) TCGA 数据挖掘和常规分析</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10">
+      <c r="A16" s="11">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1778,7 +1779,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="11">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1793,12 +1794,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从头开始的 RNA-seq 数据分析:从fastq开始质控、注释等; (2) RNA-seq 差异分析; (3) GSEA 富集分析</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10">
+      <c r="A17" s="11">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1824,7 +1825,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="11">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1839,12 +1840,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 空间转录组常规分析:大致同单细胞数据; (2) 单细胞拟时分析; (3) 单细胞注释细胞群; (4) 单细胞数据鉴定癌细胞; (5) 不同来源的 scRNA-seq 数据整合:RISC整合消除批次效应</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10">
+      <c r="A18" s="11">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1870,7 +1871,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="11">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1885,12 +1886,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 常规文献计量分析和可视化</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10">
+      <c r="A19" s="11">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1916,7 +1917,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="11">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1931,12 +1932,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等; (2) 肠道菌群和代谢物常规关联分析 (如 Pearson) :需来自于同一批样本; (3) 代谢物富集分析</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1962,7 +1963,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="11">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1982,7 +1983,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10">
+      <c r="A21" s="11">
         <v>45264</v>
       </c>
       <c r="B21">
@@ -2008,7 +2009,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="11">
         <v>45260</v>
       </c>
       <c r="H21" t="inlineStr">
@@ -2023,12 +2024,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) TCGA 数据挖掘和常规分析; (2) TCGA 变异数据挖掘和常规分析</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10">
+      <c r="A22" s="11">
         <v>45265</v>
       </c>
       <c r="B22">
@@ -2054,7 +2055,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="11">
         <v>45264</v>
       </c>
       <c r="H22" t="inlineStr">
@@ -2069,12 +2070,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 单细胞数据细胞注释到具体细胞亚群:如 Treg 细胞; (2) 单细胞细胞通讯; (3) 富集分析</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="10">
+      <c r="A23" s="11">
         <v>45272</v>
       </c>
       <c r="B23">
@@ -2100,7 +2101,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="11">
         <v>45264</v>
       </c>
       <c r="H23" t="inlineStr">
@@ -2115,12 +2116,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从 GEO 挖掘可用数据:RNA-seq; (2) RNA-seq 差异分析; (3) 富集分析; (4) 结合不同 (如疾病) 条件下 RNA-seq DEGs 筛选基因</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="10">
+      <c r="A24" s="11">
         <v>45266</v>
       </c>
       <c r="B24">
@@ -2146,7 +2147,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="11">
         <v>45266</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -2161,12 +2162,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 挖掘 HERB 数据库</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10">
+      <c r="A25" s="11">
         <v>45266</v>
       </c>
       <c r="B25">
@@ -2192,7 +2193,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="11">
         <v>45266</v>
       </c>
       <c r="H25" t="inlineStr">
@@ -2207,12 +2208,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 挖掘 HERB 数据库</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10">
+      <c r="A26" s="11">
         <v>45268</v>
       </c>
       <c r="B26">
@@ -2238,7 +2239,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="11">
         <v>45267</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -2253,12 +2254,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 挖掘 HERB 数据库</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10">
+      <c r="A27" s="11">
         <v>45275</v>
       </c>
       <c r="B27">
@@ -2284,7 +2285,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="11">
         <v>45272</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -2299,12 +2300,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) circRNA 结合 miRNA 位点预测; (2) circRNA 结合 mRNA 位点预测</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10">
+      <c r="A28" s="11">
         <v>45273</v>
       </c>
       <c r="B28">
@@ -2330,7 +2331,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="11">
         <v>45272</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -2345,12 +2346,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) RNA-seq 差异分析</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10">
+      <c r="A29" s="11">
         <v>45274</v>
       </c>
       <c r="B29">
@@ -2376,7 +2377,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="11">
         <v>45274</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -2391,12 +2392,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) RNA-seq 差异分析; (2) 富集分析</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10">
+      <c r="A30" s="11">
         <v>45295</v>
       </c>
       <c r="B30">
@@ -2422,7 +2423,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="11">
         <v>45274</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -2437,12 +2438,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) TCMSP 数据库数据挖掘; (3) 编写爬虫工具批量获取网页数据; (4) 预测化合物靶点; (5) 全自动批量分子对接; (6) 获取疾病或条件相关的基因集:Genecards</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="10">
+      <c r="A31" s="11">
         <v>45293</v>
       </c>
       <c r="B31">
@@ -2468,7 +2469,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="11">
         <v>45281</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -2483,12 +2484,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从公共数据库挖掘可用的代谢物数据; (2) 从公共数据库挖掘; (3) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (4) 蛋白质或基因和代谢物数据联合分析:通过公共数据挖掘建立联系; (5) 蛋白质或基因、肠道菌群、代谢物数据联合分析:通过公共数据; (6) 基因 (RNA) 和 eQTL 关联性挖掘:通过公共数据; (7) eQTL 和 SNP 关联性挖掘:通过公共数据; (8) SNP 和代谢物之间的关联性挖掘:通过公共数据</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="10">
+      <c r="A32" s="11">
         <v>45285</v>
       </c>
       <c r="B32">
@@ -2514,7 +2515,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="11">
         <v>45281</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -2529,12 +2530,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 挖掘 HERB 数据库; (3) 全自动批量分子对接</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10">
+      <c r="A33" s="11">
         <v>45306</v>
       </c>
       <c r="B33">
@@ -2560,7 +2561,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="11">
         <v>45288</v>
       </c>
       <c r="H33" t="inlineStr">
@@ -2575,12 +2576,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 结合不同 (如疾病) 条件下 RNA-seq DEGs 筛选基因; (2) 蛋白质与蛋白质之间的对接模拟; (3) 富集分析</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10">
+      <c r="A34" s="11">
         <v>45303</v>
       </c>
       <c r="B34">
@@ -2606,7 +2607,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="11">
         <v>45299</v>
       </c>
       <c r="H34" t="inlineStr">
@@ -2621,12 +2622,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="10">
+      <c r="A35" s="11">
         <v>45322</v>
       </c>
       <c r="B35">
@@ -2652,7 +2653,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="11">
         <v>45299</v>
       </c>
       <c r="H35" t="inlineStr">
@@ -2667,12 +2668,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 从 Plantaedb 数据库获取植物成分信息 (可能比多数中药数据库要更丰富) ; (3) 铁死亡相关基因挖掘; (4) 20% HOB 口服生物利用度预测; (5) m6A 编辑位点获取; (6) 结合不同 (如疾病) 条件下 RNA-seq DEGs 筛选基因; (7) 化合物信息获取:同义名、smiles、inchikey等; (8) 预测化合物靶点; (9) 获取疾病或条件相关的基因集:Genecards</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="10">
+      <c r="A36" s="11">
         <v>45323</v>
       </c>
       <c r="B36">
@@ -2698,7 +2699,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="11">
         <v>45302</v>
       </c>
       <c r="H36" t="inlineStr">
@@ -2713,12 +2714,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 获取疾病或条件相关的基因集:Genecards; (3) 疾病相关基因集:PharmGKB 数据库挖掘; (4) 疾病相关基因集:DisGeNet 数据库挖掘; (5) 调控该基因的相关转录因子 (TF) 数据获取; (6) 20% HOB 口服生物利用度预测; (7) 化合物系统分类注释 (ClassyFire) ; (8) 富集分析; (9) 全自动批量分子对接</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="10">
+      <c r="A37" s="11">
         <v>45322</v>
       </c>
       <c r="B37">
@@ -2744,7 +2745,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="11">
         <v>45303</v>
       </c>
       <c r="H37" t="inlineStr">
@@ -2759,12 +2760,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 编写爬虫工具批量获取网页数据</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="10">
+      <c r="A38" s="11">
         <v>45322</v>
       </c>
       <c r="B38">
@@ -2790,7 +2791,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="11">
         <v>45314</v>
       </c>
       <c r="H38" t="inlineStr">
@@ -2810,7 +2811,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="10">
+      <c r="A39" s="11">
         <v>45321</v>
       </c>
       <c r="B39">
@@ -2836,7 +2837,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="11">
         <v>45317</v>
       </c>
       <c r="H39" t="inlineStr">
@@ -2851,12 +2852,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等; (2) 从公共数据库挖掘可用的代谢物数据; (3) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (4) 蛋白质或基因和代谢物数据联合分析:通过公共数据挖掘建立联系</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="10">
+      <c r="A40" s="11">
         <v>45322</v>
       </c>
       <c r="B40">
@@ -2882,7 +2883,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="11">
         <v>45300</v>
       </c>
       <c r="H40" t="inlineStr">
@@ -2897,7 +2898,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 网络药理学; (2) 预测化合物靶点; (3) 获取疾病或条件相关的基因集:Genecards; (4) 疾病相关基因集:PharmGKB 数据库挖掘; (5) 疾病相关基因集:DisGeNet 数据库挖掘; (6) 调控该基因的相关转录因子 (TF) 数据获取; (7) 富集分析; (8) 全自动批量分子对接</t>
         </is>
       </c>
     </row>
@@ -2958,7 +2959,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="10">
+      <c r="A2" s="11">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -2984,7 +2985,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="11">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -2999,12 +3000,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 单细胞注释细胞群; (2) 单细胞拟时分析; (3) 是否昼夜节律紊乱预测:rna; (4) 单细胞细胞通讯; (5) KEGG、GO富集分析; (6) TCGA 数据挖掘和常规分析; (7) 生存分析; (8) WGCNA 共表达分析; (9) 构建 LASSO 等预测模型</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -3030,7 +3031,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="11">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -3045,12 +3046,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 从 GEO 挖掘可用数据:RNA-seq; (2) 单细胞注释细胞群; (3) 单细胞数据鉴定癌细胞; (4) 单细胞拟时分析; (5) WGCNA 共表达分析; (6) 获取疾病或条件相关的基因集:Genecards; (7) 不同来源的 scRNA-seq 数据整合:RISC整合消除批次效应; (8) 富集分析</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -3076,7 +3077,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="11">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -3091,7 +3092,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 单细胞注释细胞群; (2) 单细胞细胞通讯; (3) 不同来源的 scRNA-seq 数据整合:RISC整合消除批次效应; (4) RNA 编辑位点信息挖掘:gtex数据库etqtl挖掘; (5) 富集分析</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fri Mar  1 06:50:08 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -1063,7 +1064,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1109,7 +1110,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1135,7 +1136,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="12">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1155,7 +1156,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="12">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1181,7 +1182,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="12">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1201,7 +1202,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11">
+      <c r="A4" s="12">
         <v>45156</v>
       </c>
       <c r="B4">
@@ -1227,7 +1228,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="12">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1247,7 +1248,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11">
+      <c r="A5" s="12">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1273,7 +1274,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="12">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1293,7 +1294,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11">
+      <c r="A6" s="12">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1319,7 +1320,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="12">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1339,7 +1340,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11">
+      <c r="A7" s="12">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1365,7 +1366,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="12">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1385,7 +1386,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11">
+      <c r="A8" s="12">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1411,7 +1412,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="12">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1431,7 +1432,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11">
+      <c r="A9" s="12">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1457,7 +1458,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="12">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1477,7 +1478,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1503,7 +1504,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="12">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1523,7 +1524,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11">
+      <c r="A11" s="12">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1549,7 +1550,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="12">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1569,7 +1570,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11">
+      <c r="A12" s="12">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1595,7 +1596,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="12">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1615,7 +1616,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11">
+      <c r="A13" s="12">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1641,7 +1642,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="12">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1661,7 +1662,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11">
+      <c r="A14" s="12">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1687,7 +1688,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="12">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1707,7 +1708,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11">
+      <c r="A15" s="12">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1733,7 +1734,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="12">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1753,7 +1754,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11">
+      <c r="A16" s="12">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1779,7 +1780,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="12">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1799,7 +1800,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11">
+      <c r="A17" s="12">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1825,7 +1826,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="12">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1845,7 +1846,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11">
+      <c r="A18" s="12">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1871,7 +1872,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="12">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1891,7 +1892,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11">
+      <c r="A19" s="12">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1917,7 +1918,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="12">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1937,7 +1938,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11">
+      <c r="A20" s="12">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1963,7 +1964,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="12">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1983,7 +1984,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11">
+      <c r="A21" s="12">
         <v>45264</v>
       </c>
       <c r="B21">
@@ -2009,7 +2010,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="12">
         <v>45260</v>
       </c>
       <c r="H21" t="inlineStr">
@@ -2029,7 +2030,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="11">
+      <c r="A22" s="12">
         <v>45265</v>
       </c>
       <c r="B22">
@@ -2055,7 +2056,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="12">
         <v>45264</v>
       </c>
       <c r="H22" t="inlineStr">
@@ -2075,7 +2076,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11">
+      <c r="A23" s="12">
         <v>45272</v>
       </c>
       <c r="B23">
@@ -2101,7 +2102,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="12">
         <v>45264</v>
       </c>
       <c r="H23" t="inlineStr">
@@ -2121,7 +2122,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="11">
+      <c r="A24" s="12">
         <v>45266</v>
       </c>
       <c r="B24">
@@ -2147,7 +2148,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="12">
         <v>45266</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -2167,7 +2168,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="11">
+      <c r="A25" s="12">
         <v>45266</v>
       </c>
       <c r="B25">
@@ -2193,7 +2194,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="12">
         <v>45266</v>
       </c>
       <c r="H25" t="inlineStr">
@@ -2213,7 +2214,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="11">
+      <c r="A26" s="12">
         <v>45268</v>
       </c>
       <c r="B26">
@@ -2239,7 +2240,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="12">
         <v>45267</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -2259,7 +2260,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="11">
+      <c r="A27" s="12">
         <v>45275</v>
       </c>
       <c r="B27">
@@ -2285,7 +2286,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="12">
         <v>45272</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -2305,7 +2306,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="11">
+      <c r="A28" s="12">
         <v>45273</v>
       </c>
       <c r="B28">
@@ -2331,7 +2332,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="12">
         <v>45272</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -2351,7 +2352,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="11">
+      <c r="A29" s="12">
         <v>45274</v>
       </c>
       <c r="B29">
@@ -2377,7 +2378,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="12">
         <v>45274</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -2397,7 +2398,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="11">
+      <c r="A30" s="12">
         <v>45295</v>
       </c>
       <c r="B30">
@@ -2423,7 +2424,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="12">
         <v>45274</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -2443,7 +2444,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="11">
+      <c r="A31" s="12">
         <v>45293</v>
       </c>
       <c r="B31">
@@ -2469,7 +2470,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="12">
         <v>45281</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -2489,7 +2490,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="11">
+      <c r="A32" s="12">
         <v>45285</v>
       </c>
       <c r="B32">
@@ -2515,7 +2516,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="12">
         <v>45281</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -2535,7 +2536,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="11">
+      <c r="A33" s="12">
         <v>45306</v>
       </c>
       <c r="B33">
@@ -2561,7 +2562,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="12">
         <v>45288</v>
       </c>
       <c r="H33" t="inlineStr">
@@ -2581,8 +2582,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="11">
-        <v>45303</v>
+      <c r="A34" s="12">
+        <v>45350</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -2594,7 +2595,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>黎文华菌群+对应代谢产物介导+机制研究</t>
+          <t>414731942</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2607,7 +2608,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="12">
         <v>45299</v>
       </c>
       <c r="H34" t="inlineStr">
@@ -2622,12 +2623,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>(1) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="11">
+      <c r="A35" s="12">
         <v>45322</v>
       </c>
       <c r="B35">
@@ -2653,7 +2654,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="12">
         <v>45299</v>
       </c>
       <c r="H35" t="inlineStr">
@@ -2673,7 +2674,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="11">
+      <c r="A36" s="12">
         <v>45323</v>
       </c>
       <c r="B36">
@@ -2699,7 +2700,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="12">
         <v>45302</v>
       </c>
       <c r="H36" t="inlineStr">
@@ -2719,7 +2720,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="11">
+      <c r="A37" s="12">
         <v>45322</v>
       </c>
       <c r="B37">
@@ -2745,7 +2746,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="12">
         <v>45303</v>
       </c>
       <c r="H37" t="inlineStr">
@@ -2765,7 +2766,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="11">
+      <c r="A38" s="12">
         <v>45322</v>
       </c>
       <c r="B38">
@@ -2791,7 +2792,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="12">
         <v>45314</v>
       </c>
       <c r="H38" t="inlineStr">
@@ -2811,7 +2812,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="11">
+      <c r="A39" s="12">
         <v>45321</v>
       </c>
       <c r="B39">
@@ -2837,7 +2838,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="12">
         <v>45317</v>
       </c>
       <c r="H39" t="inlineStr">
@@ -2857,8 +2858,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="11">
-        <v>45322</v>
+      <c r="A40" s="12">
+        <v>45350</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -2870,35 +2871,541 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>414731942</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G40" s="12">
+        <v>45299</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>菌群+对应代谢产物介导+机制研究</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="12">
+        <v>45322</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>N2023121805</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>无</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>黄礼闯</t>
-        </is>
-      </c>
-      <c r="G40" s="11">
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G41" s="12">
         <v>45300</v>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>完成</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>网络药理学+Mandenol与piezo1分子对接</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t>(1) 网络药理学; (2) 预测化合物靶点; (3) 获取疾病或条件相关的基因集:Genecards; (4) 疾病相关基因集:PharmGKB 数据库挖掘; (5) 疾病相关基因集:DisGeNet 数据库挖掘; (6) 调控该基因的相关转录因子 (TF) 数据获取; (7) 富集分析; (8) 全自动批量分子对接</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>BI2024013001</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G42" s="12">
+        <v>45322</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>审核业务</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：N2024020103 02-区域-销售：张玉玲 03-上级主管：王立家 04-医院：萧山区第一人民医院 05-科室/职称：肾内科 护士长 06-电话： 07-项目（确定A/B套餐）：厅级标书+预实验 08-分值： 09-定题题目：按照技术路线图 10-时间要求：                         预实验：2024年5月30日                          标   书：2024年6月15日   11-总价： 12-定金：已付 13-评估人员 ：吴晨 14-技术支持（沟通情况）：薛富才 15-附件：报价、合同、标书申报浙江省医药科技计划、标书技术路线、预实验技术内容、技术支持与客户沟通反馈总结 16-备注： 客户要求： 1）客户分级：1.院方职务（科室职务）重点客户，做项目为了后续拿课题。 2）实验部分。在正式实验前需要进行预实验摸索动物模型建立情况，如效果好，继续做下去；效果不好，终止实验，此部分费用由我们承担。实验优先安排加急做下去，五月底做完全部实验。【预实验走实验项目】 3）标书部分。写浙江省医药科技计划标书，重点客户，安排优秀的同事写作，保证质量；6月15号前交付；如今年未立项，后续可修改一次投其他项目。 内部要求：  1）内部留存原始数据，三次重复实验 2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通【方案能调整需告知】 17-项目负责人：杨弘 </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>N2024020103</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G43" s="12">
+        <v>45324</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>筛选主动脉-下腔静脉瘘ACF模型 DEGs 并功能分析</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01-订单编号：N2024012602  02-区域-销售：江苏-郭树仁 03-上级主管：王立家 04-医院：绍兴市中 05-科室/职称：骨科 06-电话： 07-项目（确定A/B套餐）：sci1.5-2分全包B套餐 08-分值：1.5-2分 09-定题题目： 10-时间要求：2024年1月24-2025年1月24日 11-总价： 12-定金： 13-评估人员 ：林婧宇 14-技术支持（沟通情况）：薛富才-2 15-附件：合同、张春晓文章技术内容、动物伦理、动物使用许可、前期基础、申报书正文、项目计划书、客户提供数据（云附件）、技术支持与客户沟通反馈总结 16-备注： 客户要求： 1.客户分级（1.院方职务（科室职务）重点客户 2.谈单承诺：必须在时间内完成录用（2025年1月24日） 内部要求： 1)【方案能调整】方案我们定，之前内部沟通只要4月能把实验完成就行； 2)需要安排外部投稿； @助理陈芳媛 3)全包实验，尽量按实验数据交付。 4）内部留存原始数据，三次重复实验 17-项目负责人：杨啸   </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>N2024012602</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1.5-2分</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G44" s="12">
+        <v>45324</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Hydroxysafflor Yellow A 与Piezo1对接</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号：N2024010303【方案能调整需告知】 02-区域-销售：张玉玲 03-上级主管：王立家 04-医院： 05-科室/职称：儿科 正高  科主任 06-电话： 07-项目（确定A/B套餐）：中管局标书（实验走实验项目 08-分值： 09-定题题目：按照技术路线 10-时间要求：2024年6月10日 11-总价： 12-定金： 13-评估人员 ：吴晨 14-技术支持（沟通情况）：薛富才，龙艳 15-附件：技术支持与客户沟通反馈总结、技术路线，技术内容、（报价，预实验报价、合同、客户提供的前期研究基础等资料见压缩包）16-备注：客户要求：1）客户分级：重点客户，做项目为了后续拿课题。 2）谈单承诺：实验部分需要加急安排做！重点客户，根据方案设计写中管局标书，需要2024年6月10日前交付！辛苦安排优秀的同事写，质量要高。 内部要求：1）内部留存原始数据，三次重复实验2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通； 17-项目负责人：杨啸 </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>N2024010303</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G45" s="12">
+        <v>45326</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>分子对接 Celogenamide A（环状肽）蛋白 SSTR2</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>20231012</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G46" s="12">
+        <v>45343</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>建立风险模型和作图</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>20230815</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G47" s="12">
+        <v>45344</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>列线图模型建立与验证</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="12">
+        <v>45350</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号：N2024022202  02-区域-销售：浙江台州-吴航贵 03-上级主管：王立家 04-医院：温岭市第一人民医院 05-科室/职称：肝病科/科主任 06-电话： 07-项目（确定A/B套餐）： 08-分值： 09-定题题目：乙肝病毒HBx利用泛素化系统降解XXX上调YYY诱导肝癌线粒体自噬的机制研究【方案不能调整】 10-时间要求：2024年2月22日--2024年06月15日 11-总价： 12-定金： 13-评估人员 ： 14-技术支持（沟通情况）：薛富才，吴晨（沟通次数）3次， 15-附件：标书技术路线、预实验技术内容、技术支持与客户沟通反馈总结、合同、预实验报价 16-备注： 客户要求： 1）客户分级：1.院方职务(科室职务)重点客户，做项目为了后续拿课题 2）尽量在今年省自然投之前给到客户交付 内部要求： 1）内部留存原始数据，三次重复实验 ；  2）方案不能调整； 3）预实验走实验项目 17-项目负责人：杨啸 </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>N2024022202</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G48" s="12">
+        <v>45345</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>乙肝病毒HBx利用泛素化系统降解XXX上调YYY诱导肝癌线粒体自噬</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="12">
+        <v>45351</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>workflow</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G49" s="12">
+        <v>45351</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Step 系列：scRNA-seq 基本分析</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="12">
+        <v>45351</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>workflow</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G50" s="12">
+        <v>45351</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Step 系列：Prologue and Get-start</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="12">
+        <v>45351</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>workflow</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G51" s="12">
+        <v>45351</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Step 系列：scRNA-seq 癌细胞鉴定</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
@@ -2959,7 +3466,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -2985,7 +3492,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="12">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -3005,7 +3512,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="12">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -3031,7 +3538,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="12">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -3051,7 +3558,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11">
+      <c r="A4" s="12">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -3077,7 +3584,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="12">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Fri Mar 29 06:50:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -1064,7 +1065,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1110,7 +1111,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="12">
+      <c r="A2" s="13">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1136,7 +1137,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="13">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1156,7 +1157,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12">
+      <c r="A3" s="13">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1182,7 +1183,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="13">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1202,7 +1203,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <v>45156</v>
       </c>
       <c r="B4">
@@ -1228,7 +1229,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="13">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1248,7 +1249,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12">
+      <c r="A5" s="13">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1274,7 +1275,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="13">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1294,7 +1295,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1320,7 +1321,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="13">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1340,7 +1341,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12">
+      <c r="A7" s="13">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1366,7 +1367,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="13">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1386,7 +1387,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1412,7 +1413,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="13">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1432,7 +1433,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1458,7 +1459,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="13">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1478,7 +1479,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12">
+      <c r="A10" s="13">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1504,7 +1505,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="13">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1524,7 +1525,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12">
+      <c r="A11" s="13">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1550,7 +1551,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="13">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1570,7 +1571,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1596,7 +1597,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="13">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1616,7 +1617,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1642,7 +1643,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="13">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1662,7 +1663,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1688,7 +1689,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="13">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1708,7 +1709,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12">
+      <c r="A15" s="13">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1734,7 +1735,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="13">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1754,7 +1755,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12">
+      <c r="A16" s="13">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1780,7 +1781,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="13">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1800,7 +1801,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12">
+      <c r="A17" s="13">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1826,7 +1827,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="13">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1846,7 +1847,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1872,7 +1873,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="13">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1892,7 +1893,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12">
+      <c r="A19" s="13">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1918,7 +1919,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="13">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1938,7 +1939,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12">
+      <c r="A20" s="13">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1964,7 +1965,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="13">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1984,7 +1985,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12">
+      <c r="A21" s="13">
         <v>45264</v>
       </c>
       <c r="B21">
@@ -2010,7 +2011,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="13">
         <v>45260</v>
       </c>
       <c r="H21" t="inlineStr">
@@ -2030,7 +2031,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>45265</v>
       </c>
       <c r="B22">
@@ -2056,7 +2057,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="13">
         <v>45264</v>
       </c>
       <c r="H22" t="inlineStr">
@@ -2076,7 +2077,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12">
+      <c r="A23" s="13">
         <v>45272</v>
       </c>
       <c r="B23">
@@ -2102,7 +2103,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="13">
         <v>45264</v>
       </c>
       <c r="H23" t="inlineStr">
@@ -2122,7 +2123,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12">
+      <c r="A24" s="13">
         <v>45266</v>
       </c>
       <c r="B24">
@@ -2148,7 +2149,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="13">
         <v>45266</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -2168,7 +2169,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12">
+      <c r="A25" s="13">
         <v>45266</v>
       </c>
       <c r="B25">
@@ -2194,7 +2195,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="13">
         <v>45266</v>
       </c>
       <c r="H25" t="inlineStr">
@@ -2214,7 +2215,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12">
+      <c r="A26" s="13">
         <v>45268</v>
       </c>
       <c r="B26">
@@ -2240,7 +2241,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="13">
         <v>45267</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -2260,7 +2261,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="12">
+      <c r="A27" s="13">
         <v>45275</v>
       </c>
       <c r="B27">
@@ -2286,7 +2287,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="13">
         <v>45272</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -2306,7 +2307,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="12">
+      <c r="A28" s="13">
         <v>45273</v>
       </c>
       <c r="B28">
@@ -2332,7 +2333,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="13">
         <v>45272</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -2352,7 +2353,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="12">
+      <c r="A29" s="13">
         <v>45274</v>
       </c>
       <c r="B29">
@@ -2378,7 +2379,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="13">
         <v>45274</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -2398,8 +2399,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="12">
-        <v>45295</v>
+      <c r="A30" s="13">
+        <v>45359</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -2424,7 +2425,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="13">
         <v>45274</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -2444,7 +2445,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="12">
+      <c r="A31" s="13">
         <v>45293</v>
       </c>
       <c r="B31">
@@ -2470,7 +2471,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="13">
         <v>45281</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -2490,7 +2491,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="12">
+      <c r="A32" s="13">
         <v>45285</v>
       </c>
       <c r="B32">
@@ -2516,7 +2517,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="13">
         <v>45281</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -2536,7 +2537,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="12">
+      <c r="A33" s="13">
         <v>45306</v>
       </c>
       <c r="B33">
@@ -2562,7 +2563,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="13">
         <v>45288</v>
       </c>
       <c r="H33" t="inlineStr">
@@ -2582,8 +2583,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="12">
-        <v>45350</v>
+      <c r="A34" s="13">
+        <v>45363</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -2595,7 +2596,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>414731942</t>
+          <t>黎文华订单</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2608,7 +2609,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="13">
         <v>45299</v>
       </c>
       <c r="H34" t="inlineStr">
@@ -2628,7 +2629,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="12">
+      <c r="A35" s="13">
         <v>45322</v>
       </c>
       <c r="B35">
@@ -2654,7 +2655,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="13">
         <v>45299</v>
       </c>
       <c r="H35" t="inlineStr">
@@ -2674,7 +2675,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="12">
+      <c r="A36" s="13">
         <v>45323</v>
       </c>
       <c r="B36">
@@ -2700,7 +2701,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="13">
         <v>45302</v>
       </c>
       <c r="H36" t="inlineStr">
@@ -2720,7 +2721,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="12">
+      <c r="A37" s="13">
         <v>45322</v>
       </c>
       <c r="B37">
@@ -2746,7 +2747,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="13">
         <v>45303</v>
       </c>
       <c r="H37" t="inlineStr">
@@ -2766,7 +2767,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="12">
+      <c r="A38" s="13">
         <v>45322</v>
       </c>
       <c r="B38">
@@ -2792,7 +2793,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G38" s="12">
+      <c r="G38" s="13">
         <v>45314</v>
       </c>
       <c r="H38" t="inlineStr">
@@ -2812,7 +2813,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="12">
+      <c r="A39" s="13">
         <v>45321</v>
       </c>
       <c r="B39">
@@ -2838,7 +2839,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="13">
         <v>45317</v>
       </c>
       <c r="H39" t="inlineStr">
@@ -2858,8 +2859,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="12">
-        <v>45350</v>
+      <c r="A40" s="13">
+        <v>45363</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -2871,7 +2872,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>414731942</t>
+          <t>黎文华订单</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2884,7 +2885,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="13">
         <v>45299</v>
       </c>
       <c r="H40" t="inlineStr">
@@ -2904,7 +2905,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="12">
+      <c r="A41" s="13">
         <v>45322</v>
       </c>
       <c r="B41">
@@ -2930,7 +2931,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="13">
         <v>45300</v>
       </c>
       <c r="H41" t="inlineStr">
@@ -2950,7 +2951,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="12">
+      <c r="A42" s="13">
         <v>45350</v>
       </c>
       <c r="B42">
@@ -2976,7 +2977,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="13">
         <v>45322</v>
       </c>
       <c r="H42" t="inlineStr">
@@ -2996,7 +2997,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="12">
+      <c r="A43" s="13">
         <v>45350</v>
       </c>
       <c r="B43">
@@ -3022,7 +3023,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="13">
         <v>45324</v>
       </c>
       <c r="H43" t="inlineStr">
@@ -3042,7 +3043,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="12">
+      <c r="A44" s="13">
         <v>45350</v>
       </c>
       <c r="B44">
@@ -3068,7 +3069,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="13">
         <v>45324</v>
       </c>
       <c r="H44" t="inlineStr">
@@ -3088,7 +3089,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="12">
+      <c r="A45" s="13">
         <v>45350</v>
       </c>
       <c r="B45">
@@ -3114,7 +3115,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="13">
         <v>45326</v>
       </c>
       <c r="H45" t="inlineStr">
@@ -3134,8 +3135,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="12">
-        <v>45350</v>
+      <c r="A46" s="13">
+        <v>45351</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -3160,7 +3161,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G46" s="12">
+      <c r="G46" s="13">
         <v>45343</v>
       </c>
       <c r="H46" t="inlineStr">
@@ -3180,8 +3181,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="12">
-        <v>45350</v>
+      <c r="A47" s="13">
+        <v>45352</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -3206,7 +3207,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G47" s="12">
+      <c r="G47" s="13">
         <v>45344</v>
       </c>
       <c r="H47" t="inlineStr">
@@ -3226,8 +3227,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="12">
-        <v>45350</v>
+      <c r="A48" s="13">
+        <v>45351</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -3252,7 +3253,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G48" s="12">
+      <c r="G48" s="13">
         <v>45345</v>
       </c>
       <c r="H48" t="inlineStr">
@@ -3272,7 +3273,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="12">
+      <c r="A49" s="13">
         <v>45351</v>
       </c>
       <c r="B49">
@@ -3298,7 +3299,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G49" s="12">
+      <c r="G49" s="13">
         <v>45351</v>
       </c>
       <c r="H49" t="inlineStr">
@@ -3318,7 +3319,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="12">
+      <c r="A50" s="13">
         <v>45351</v>
       </c>
       <c r="B50">
@@ -3344,7 +3345,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G50" s="12">
+      <c r="G50" s="13">
         <v>45351</v>
       </c>
       <c r="H50" t="inlineStr">
@@ -3364,7 +3365,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="12">
+      <c r="A51" s="13">
         <v>45351</v>
       </c>
       <c r="B51">
@@ -3390,7 +3391,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G51" s="12">
+      <c r="G51" s="13">
         <v>45351</v>
       </c>
       <c r="H51" t="inlineStr">
@@ -3404,6 +3405,558 @@
         </is>
       </c>
       <c r="J51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="13">
+        <v>45359</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>筛选差异蛋白和对应配体蛋白</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G52" s="13">
+        <v>45344</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>筛选差异蛋白和对应配体蛋白</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="13">
+        <v>45355</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>审核业务</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G53" s="13">
+        <v>45345</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>审核业务</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="13">
+        <v>45363</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号：2024010202  02-代理：唐丽娟 03-客户：高杰 04-单位： 05-科室/职称： 06-项目：sci0-1，临床 07-分值：0-1分 08-题目：冠心病患者术后心律失常的危险因素分析及列线图风险模型建立 09-时间要求：2024年6月30日（3-6个月录用） 10-总价： 11-定金：已付 12-评估： 13-备注：走朱总定向杂志@芳媛，辛苦评估，谢谢~ </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2024010202</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0-1分，临床</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G54" s="13">
+        <v>45351</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>建立风险模型</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="13">
+        <v>45356</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>N2023121508</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G55" s="13">
+        <v>45355</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Sepsis差异代谢物和热图绘制</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="13">
+        <v>45369</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>结肠炎和结肠癌的差异菌群</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G56" s="13">
+        <v>45355</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>结肠炎和结肠癌的差异菌群</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="13">
+        <v>45357</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>N2023121401</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G57" s="13">
+        <v>45356</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>网络药理学寻找复方的靶点通路</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="13">
+        <v>45378</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>S2023102503</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G58" s="13">
+        <v>45359</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>VASH2 序列分析</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="13">
+        <v>45366</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>养阴通脑颗粒中关键成分对脑缺血再灌注的影响</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G59" s="13">
+        <v>45364</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>养阴通脑颗粒中关键成分对脑缺血再灌注的影响</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="13">
+        <v>45379</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号： IN2024031807 02-区域-销售：张玉玲 03-上级主管：王立家 04-医院： 05-科室/职称：icu 副高 06-电话： 07-项目（确定A/B套餐）： 生信分析 08-分值： 09-定题题目： 10-时间要求：2024年3月13日——2024年4月13日  11-总价： 12-定金：已付 13-评估人员 ：吴晨 14-技术支持（沟通情况）：吴晨，薛富才 15-附件： 技术支持与客户沟通反馈总结（word)、合同  16-备注：   16.1客户分级：1.院方职务（科室职务）重点客户，做项目为了后续拿课题。   16.2生信分析需求：网络药理学分析参苓白术散治治疗脓毒症肠损伤的药物活性成分XXX，对接下游的靶点YYY（表观遗传学修饰蛋白）， YYY可以对靶点ZZZ进行表观遗传学修饰。YYY-ZZZ的机制和调控脓毒症肠损伤相关。 【方案能调整】 16.3谈单承诺： 客户要求一个月内结果给到客户，如超期尾款将少收2000 17-项目负责人：杨啸 </t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>IN2024031807</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G60" s="13">
+        <v>45370</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>网络药理学和表观遗传学修饰筛选靶点</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="13">
+        <v>45376</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>雅威审核</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G61" s="13">
+        <v>45374</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>雅威审核</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="13">
+        <v>45379</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>戴心怡沟通</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G62" s="13">
+        <v>45379</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="13">
+        <v>45379</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号： SCI：N2024032701、中管局标书：N2024032702、卫生厅标书：N2024032703、省自然标书：N2024032704  02-区域-销售：孟珏 03-上级主管：张玉玲 04-医院： 05-科室/职称：肛肠外科主治 06-电话： 07-项目（确定A/B套餐）：B套餐 08-分值：中科院三区3-5 分 09-定题题目：中药复方(乌梅丸)及活性成分XXX调控肠上皮细胞与成纤维细胞串扰干预炎性肠病的作用和机制研究（文章不含中药复方的实验，题目可以把其去掉，详见附件:“技术支持与客户沟通反馈总结V2”） 10-时间要求：中管局标书、卫生厅标书： 2024年6月    省自然标书：预计2025年申请     中科院三区3-5 分SCI：2026年3月15日   11-总价：（以合同为准） 12-定金：已付 13-评估人员 ：吴晨 14-技术支持（沟通情况）：薛富才 15-附件：实验报价、合同、技术路线、 技术内容、技术支持与客户沟通反馈总结 16-备注： 客户要求： 1）客户分级：潜力客户，做项目为了后续拿课题 2）需要加急做实验，能做多少做多少，中管局和卫生厅的标书先写起来，实验有一部分结果出来了就写到标书中。客户要今年先申报上去试试。 3）客户总共三个标书，中管局，卫生厅，省自然。目前需要做中管局和卫生厅，省自然不那么急。以往卫生厅，中管局标书六月交。 4）项目周期两年，预实验走全包实验，实验结果按阶段交付； 5）附件“齐海鑫-技术实验报价V3”是补充的报价表，将全包文章中做预实验的部分价格和实验周期单独列出来了。（卫生厅预实验中标红的费用，是与全包文章中有重复计算的部分） 6）中管局和卫生厅课题的预实验已在技术内容中标出。省自然预实验建议和中管局用同样的预实验即可。 内部要求：   1）内部留存原始数据，三次重复实验 ； 2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通； 3）实验分类的时候，WB备注一下整张膜带marker，流式需要有fcs格式文件； 17-项目与负责人：杨啸 </t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>N2024032701</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>中科院三区3-5 分</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G63" s="13">
+        <v>45378</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>中药复方乌梅丸网络药理学分析</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3466,7 +4019,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="12">
+      <c r="A2" s="13">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -3492,7 +4045,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="13">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -3512,7 +4065,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12">
+      <c r="A3" s="13">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -3538,7 +4091,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="13">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -3558,7 +4111,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -3584,7 +4137,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="13">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Tue Apr 30 06:50:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,7 +698,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -708,6 +708,7 @@
     <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -1065,7 +1066,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1111,7 +1112,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="13">
+      <c r="A2" s="14">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1137,7 +1138,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="14">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1157,7 +1158,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1183,7 +1184,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="14">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1203,7 +1204,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>45156</v>
       </c>
       <c r="B4">
@@ -1229,7 +1230,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="14">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1249,7 +1250,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1275,7 +1276,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1295,7 +1296,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1321,7 +1322,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="14">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1341,7 +1342,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13">
+      <c r="A7" s="14">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1367,7 +1368,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1387,7 +1388,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1413,7 +1414,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="14">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1433,7 +1434,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1459,7 +1460,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="14">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1479,7 +1480,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1505,7 +1506,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="14">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1525,7 +1526,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13">
+      <c r="A11" s="14">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1551,7 +1552,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="14">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1571,7 +1572,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1597,7 +1598,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="14">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1617,7 +1618,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="13">
+      <c r="A13" s="14">
         <v>45216</v>
       </c>
       <c r="B13">
@@ -1643,7 +1644,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="14">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1663,7 +1664,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13">
+      <c r="A14" s="14">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1689,7 +1690,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="14">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1709,7 +1710,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13">
+      <c r="A15" s="14">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1735,7 +1736,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="14">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1755,7 +1756,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="14">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1781,7 +1782,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="14">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1801,7 +1802,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13">
+      <c r="A17" s="14">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1827,7 +1828,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="14">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1847,7 +1848,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="13">
+      <c r="A18" s="14">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1873,7 +1874,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="14">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1893,7 +1894,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="13">
+      <c r="A19" s="14">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1919,7 +1920,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1939,7 +1940,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1965,7 +1966,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="14">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1985,7 +1986,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="13">
+      <c r="A21" s="14">
         <v>45264</v>
       </c>
       <c r="B21">
@@ -2011,7 +2012,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="14">
         <v>45260</v>
       </c>
       <c r="H21" t="inlineStr">
@@ -2031,7 +2032,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="13">
+      <c r="A22" s="14">
         <v>45265</v>
       </c>
       <c r="B22">
@@ -2057,7 +2058,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <v>45264</v>
       </c>
       <c r="H22" t="inlineStr">
@@ -2077,7 +2078,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="13">
+      <c r="A23" s="14">
         <v>45272</v>
       </c>
       <c r="B23">
@@ -2103,7 +2104,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="14">
         <v>45264</v>
       </c>
       <c r="H23" t="inlineStr">
@@ -2123,7 +2124,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>45266</v>
       </c>
       <c r="B24">
@@ -2149,7 +2150,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="14">
         <v>45266</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -2169,7 +2170,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="13">
+      <c r="A25" s="14">
         <v>45266</v>
       </c>
       <c r="B25">
@@ -2195,7 +2196,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="14">
         <v>45266</v>
       </c>
       <c r="H25" t="inlineStr">
@@ -2215,7 +2216,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13">
+      <c r="A26" s="14">
         <v>45268</v>
       </c>
       <c r="B26">
@@ -2241,7 +2242,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="14">
         <v>45267</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -2261,7 +2262,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>45275</v>
       </c>
       <c r="B27">
@@ -2287,7 +2288,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="14">
         <v>45272</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -2307,7 +2308,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>45273</v>
       </c>
       <c r="B28">
@@ -2333,7 +2334,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="14">
         <v>45272</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -2353,7 +2354,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="13">
+      <c r="A29" s="14">
         <v>45274</v>
       </c>
       <c r="B29">
@@ -2379,7 +2380,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="14">
         <v>45274</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -2399,7 +2400,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>45359</v>
       </c>
       <c r="B30">
@@ -2425,7 +2426,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="14">
         <v>45274</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -2445,7 +2446,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="13">
+      <c r="A31" s="14">
         <v>45293</v>
       </c>
       <c r="B31">
@@ -2471,7 +2472,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="14">
         <v>45281</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -2491,7 +2492,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="13">
+      <c r="A32" s="14">
         <v>45285</v>
       </c>
       <c r="B32">
@@ -2517,7 +2518,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="14">
         <v>45281</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -2537,7 +2538,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="13">
+      <c r="A33" s="14">
         <v>45306</v>
       </c>
       <c r="B33">
@@ -2563,7 +2564,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="14">
         <v>45288</v>
       </c>
       <c r="H33" t="inlineStr">
@@ -2583,7 +2584,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="13">
+      <c r="A34" s="14">
         <v>45363</v>
       </c>
       <c r="B34">
@@ -2609,7 +2610,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="14">
         <v>45299</v>
       </c>
       <c r="H34" t="inlineStr">
@@ -2629,7 +2630,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="13">
+      <c r="A35" s="14">
         <v>45322</v>
       </c>
       <c r="B35">
@@ -2655,7 +2656,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="14">
         <v>45299</v>
       </c>
       <c r="H35" t="inlineStr">
@@ -2675,7 +2676,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="13">
+      <c r="A36" s="14">
         <v>45323</v>
       </c>
       <c r="B36">
@@ -2701,7 +2702,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="14">
         <v>45302</v>
       </c>
       <c r="H36" t="inlineStr">
@@ -2721,7 +2722,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="13">
+      <c r="A37" s="14">
         <v>45322</v>
       </c>
       <c r="B37">
@@ -2747,7 +2748,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="14">
         <v>45303</v>
       </c>
       <c r="H37" t="inlineStr">
@@ -2767,7 +2768,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="13">
+      <c r="A38" s="14">
         <v>45322</v>
       </c>
       <c r="B38">
@@ -2793,7 +2794,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="14">
         <v>45314</v>
       </c>
       <c r="H38" t="inlineStr">
@@ -2813,7 +2814,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="13">
+      <c r="A39" s="14">
         <v>45321</v>
       </c>
       <c r="B39">
@@ -2839,7 +2840,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G39" s="13">
+      <c r="G39" s="14">
         <v>45317</v>
       </c>
       <c r="H39" t="inlineStr">
@@ -2859,7 +2860,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="13">
+      <c r="A40" s="14">
         <v>45363</v>
       </c>
       <c r="B40">
@@ -2885,7 +2886,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G40" s="13">
+      <c r="G40" s="14">
         <v>45299</v>
       </c>
       <c r="H40" t="inlineStr">
@@ -2905,7 +2906,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="13">
+      <c r="A41" s="14">
         <v>45322</v>
       </c>
       <c r="B41">
@@ -2931,7 +2932,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="14">
         <v>45300</v>
       </c>
       <c r="H41" t="inlineStr">
@@ -2951,7 +2952,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="13">
+      <c r="A42" s="14">
         <v>45350</v>
       </c>
       <c r="B42">
@@ -2977,7 +2978,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G42" s="13">
+      <c r="G42" s="14">
         <v>45322</v>
       </c>
       <c r="H42" t="inlineStr">
@@ -2997,7 +2998,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="13">
+      <c r="A43" s="14">
         <v>45350</v>
       </c>
       <c r="B43">
@@ -3023,7 +3024,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="14">
         <v>45324</v>
       </c>
       <c r="H43" t="inlineStr">
@@ -3043,7 +3044,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="13">
+      <c r="A44" s="14">
         <v>45350</v>
       </c>
       <c r="B44">
@@ -3069,7 +3070,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="14">
         <v>45324</v>
       </c>
       <c r="H44" t="inlineStr">
@@ -3089,7 +3090,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="13">
+      <c r="A45" s="14">
         <v>45350</v>
       </c>
       <c r="B45">
@@ -3115,7 +3116,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="14">
         <v>45326</v>
       </c>
       <c r="H45" t="inlineStr">
@@ -3135,7 +3136,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="13">
+      <c r="A46" s="14">
         <v>45351</v>
       </c>
       <c r="B46">
@@ -3161,7 +3162,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="14">
         <v>45343</v>
       </c>
       <c r="H46" t="inlineStr">
@@ -3181,7 +3182,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="13">
+      <c r="A47" s="14">
         <v>45352</v>
       </c>
       <c r="B47">
@@ -3207,7 +3208,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="14">
         <v>45344</v>
       </c>
       <c r="H47" t="inlineStr">
@@ -3227,7 +3228,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="13">
+      <c r="A48" s="14">
         <v>45351</v>
       </c>
       <c r="B48">
@@ -3253,7 +3254,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="14">
         <v>45345</v>
       </c>
       <c r="H48" t="inlineStr">
@@ -3273,7 +3274,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="13">
+      <c r="A49" s="14">
         <v>45351</v>
       </c>
       <c r="B49">
@@ -3299,7 +3300,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="14">
         <v>45351</v>
       </c>
       <c r="H49" t="inlineStr">
@@ -3319,7 +3320,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="13">
+      <c r="A50" s="14">
         <v>45351</v>
       </c>
       <c r="B50">
@@ -3345,7 +3346,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="14">
         <v>45351</v>
       </c>
       <c r="H50" t="inlineStr">
@@ -3365,7 +3366,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="13">
+      <c r="A51" s="14">
         <v>45351</v>
       </c>
       <c r="B51">
@@ -3391,7 +3392,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="14">
         <v>45351</v>
       </c>
       <c r="H51" t="inlineStr">
@@ -3411,8 +3412,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="13">
-        <v>45359</v>
+      <c r="A52" s="14">
+        <v>45406</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -3437,7 +3438,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G52" s="13">
+      <c r="G52" s="14">
         <v>45344</v>
       </c>
       <c r="H52" t="inlineStr">
@@ -3457,7 +3458,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="13">
+      <c r="A53" s="14">
         <v>45355</v>
       </c>
       <c r="B53">
@@ -3483,7 +3484,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="14">
         <v>45345</v>
       </c>
       <c r="H53" t="inlineStr">
@@ -3503,7 +3504,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="13">
+      <c r="A54" s="14">
         <v>45363</v>
       </c>
       <c r="B54">
@@ -3529,7 +3530,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G54" s="13">
+      <c r="G54" s="14">
         <v>45351</v>
       </c>
       <c r="H54" t="inlineStr">
@@ -3549,7 +3550,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="13">
+      <c r="A55" s="14">
         <v>45356</v>
       </c>
       <c r="B55">
@@ -3575,7 +3576,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G55" s="13">
+      <c r="G55" s="14">
         <v>45355</v>
       </c>
       <c r="H55" t="inlineStr">
@@ -3595,7 +3596,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="13">
+      <c r="A56" s="14">
         <v>45369</v>
       </c>
       <c r="B56">
@@ -3621,7 +3622,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G56" s="13">
+      <c r="G56" s="14">
         <v>45355</v>
       </c>
       <c r="H56" t="inlineStr">
@@ -3641,7 +3642,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="13">
+      <c r="A57" s="14">
         <v>45357</v>
       </c>
       <c r="B57">
@@ -3667,7 +3668,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="14">
         <v>45356</v>
       </c>
       <c r="H57" t="inlineStr">
@@ -3687,7 +3688,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="13">
+      <c r="A58" s="14">
         <v>45378</v>
       </c>
       <c r="B58">
@@ -3713,7 +3714,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="14">
         <v>45359</v>
       </c>
       <c r="H58" t="inlineStr">
@@ -3733,7 +3734,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="13">
+      <c r="A59" s="14">
         <v>45366</v>
       </c>
       <c r="B59">
@@ -3759,7 +3760,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G59" s="13">
+      <c r="G59" s="14">
         <v>45364</v>
       </c>
       <c r="H59" t="inlineStr">
@@ -3779,7 +3780,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="13">
+      <c r="A60" s="14">
         <v>45379</v>
       </c>
       <c r="B60">
@@ -3805,7 +3806,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G60" s="13">
+      <c r="G60" s="14">
         <v>45370</v>
       </c>
       <c r="H60" t="inlineStr">
@@ -3825,7 +3826,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="13">
+      <c r="A61" s="14">
         <v>45376</v>
       </c>
       <c r="B61">
@@ -3851,7 +3852,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G61" s="13">
+      <c r="G61" s="14">
         <v>45374</v>
       </c>
       <c r="H61" t="inlineStr">
@@ -3871,7 +3872,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="13">
+      <c r="A62" s="14">
         <v>45379</v>
       </c>
       <c r="B62">
@@ -3897,7 +3898,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="14">
         <v>45379</v>
       </c>
       <c r="H62" t="inlineStr">
@@ -3917,46 +3918,460 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="13">
-        <v>45379</v>
+      <c r="A63" s="14">
+        <v>45406</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>筛选差异蛋白和对应配体蛋白</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G63" s="14">
+        <v>45344</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>筛选差异蛋白和对应配体蛋白</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="14">
+        <v>45401</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t xml:space="preserve">01-订单编号： SCI：N2024032701、中管局标书：N2024032702、卫生厅标书：N2024032703、省自然标书：N2024032704  02-区域-销售：孟珏 03-上级主管：张玉玲 04-医院： 05-科室/职称：肛肠外科主治 06-电话： 07-项目（确定A/B套餐）：B套餐 08-分值：中科院三区3-5 分 09-定题题目：中药复方(乌梅丸)及活性成分XXX调控肠上皮细胞与成纤维细胞串扰干预炎性肠病的作用和机制研究（文章不含中药复方的实验，题目可以把其去掉，详见附件:“技术支持与客户沟通反馈总结V2”） 10-时间要求：中管局标书、卫生厅标书： 2024年6月    省自然标书：预计2025年申请     中科院三区3-5 分SCI：2026年3月15日   11-总价：（以合同为准） 12-定金：已付 13-评估人员 ：吴晨 14-技术支持（沟通情况）：薛富才 15-附件：实验报价、合同、技术路线、 技术内容、技术支持与客户沟通反馈总结 16-备注： 客户要求： 1）客户分级：潜力客户，做项目为了后续拿课题 2）需要加急做实验，能做多少做多少，中管局和卫生厅的标书先写起来，实验有一部分结果出来了就写到标书中。客户要今年先申报上去试试。 3）客户总共三个标书，中管局，卫生厅，省自然。目前需要做中管局和卫生厅，省自然不那么急。以往卫生厅，中管局标书六月交。 4）项目周期两年，预实验走全包实验，实验结果按阶段交付； 5）附件“齐海鑫-技术实验报价V3”是补充的报价表，将全包文章中做预实验的部分价格和实验周期单独列出来了。（卫生厅预实验中标红的费用，是与全包文章中有重复计算的部分） 6）中管局和卫生厅课题的预实验已在技术内容中标出。省自然预实验建议和中管局用同样的预实验即可。 内部要求：   1）内部留存原始数据，三次重复实验 ； 2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通； 3）实验分类的时候，WB备注一下整张膜带marker，流式需要有fcs格式文件； 17-项目与负责人：杨啸 </t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>N2024032701</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>中科院三区3-5 分</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>黄礼闯</t>
-        </is>
-      </c>
-      <c r="G63" s="13">
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G64" s="14">
         <v>45378</v>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>完成</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
         <is>
           <t>中药复方乌梅丸网络药理学分析</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="J64" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="14">
+        <v>45389</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>三阴乳腺癌的多药耐药的靶点分析</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G65" s="14">
+        <v>45384</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>三阴乳腺癌的多药耐药的靶点分析</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="14">
+        <v>45407</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>N2024022202</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G66" s="14">
+        <v>45384</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>确定HBX的CDS区序列</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="14">
+        <v>45401</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号： N2024040301  02-区域-销售：金华\邱海玉 03-上级主管：张玉玲 04-医院：金华市人民医院 05-科室/职称：风湿免疫科/副高 06-电话： 07-项目（确定A/B套餐）：市厅级标书【预实验走全包】 08-分值： 09-定题题目： XX通过有氧糖酵解调控巨噬细胞极性治疗类风湿性关节炎 10-时间要求：2024年8月29日 11-总价： 12-定金：已付 13-评估人员 ：林婧宇 14-技术支持（沟通情况）：林婧宇，薛富才 15-附件：预实验报价、合同、技术路线、预实验方案、技术支持与客户沟通反馈总结 16-备注： 客户要求： 1）客户分级：潜力客户 2）如果客户课题未中，需要根据卫生厅反馈意见修改 ； 3）实验需要按实验项目交付，实验结果尽量多给到客户，阴性结果和阳性结果多拍些图片，不管好的或者不好的结果 内部要求： 1）内部留存原始数据，三次重复实验 2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通【方案能调整】； 17-项目负责人：杨啸 </t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>N2024040301</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G67" s="14">
+        <v>45385</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>XX基因通过促进糖酵解促进巨噬细胞M1极化</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="14">
+        <v>45399</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号： A2024040307  02-区域-销售：郭树仁 03-上级主管：王立家 04-医院： 05-科室/职称：心胸 06-电话： 07-项目（确定A/B套餐）：sci3-5 分全包A套餐 08-分值：3-5 分 09-定题题目： XX（FKBP5）乙酰化调控心肌梗死（血栓导致）后的心房炎症和纤维化的作用机制 10-时间要求：SCI：2026年3月25日（实验需要12个月内完成） 11-总价： 12-定金：已付 13-评估人员 ：林靖宇 14-技术支持（沟通情况）：薛富才（3） 15-附件：实验报价 、合同、技术支持与客户沟通反馈总结、技术路线、客户资料  16-备注： 客户要求： 1）谈单承诺：需加急尽快完成，设计方案时候已经确认过，12个月内需要完成实验、客户要求每月学生去实验室1-2次，差旅费公司报销，需要阶段性报告 2）实验走实验项目，学生参与学习实验操作。按合同分阶段汇报实验结果。 内部要求： 1）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通【方案能调整】； 2）实验走实验项目，内部留存原始数据，三次重复实验； 3）实验分类的时候，WB备注一下整张膜带marker，流式需要有fcs格式文件  17-项目负责人：杨弘 </t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>A2024040307</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>3-5 分</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G68" s="14">
+        <v>45389</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>乙酰化酶分析筛选</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="14">
+        <v>45392</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>蛋白质数据绘制火山图</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G69" s="14">
+        <v>45391</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>蛋白质数据绘制火山图</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="14">
+        <v>45399</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号：卫生厅标书单号：N2024031302      中管局标书单号：N2024031303（在N2024031302方案基础上稍作调整） 02-区域-销售：杭州-付梓欣 03-上级领导：王立家 04-医院：富阳区人民医院 05-科室/职称：中医科／主任 06-电话： 07-项目（确定A/B套餐）： 卫生厅标书 +中管局标书  08-分值： 09-定题题目：祛瘀解毒类中药通过调控炎症信号通路介导肿瘤免疫微环境抑制乳腺癌的机制研究 10-时间要求： 实验：2024年3月1日—2024年11月30日                                     卫生厅标书：2024年11月30日—2025年2月28日                        中管局标书：2024年11月30日—2025年2月28日 12-定金：已付 13-评估人员 ： 14-技术支持（沟通情况）：林靖宇 15-附件：技术路线、实验报价、预实验方案、实验合同、技术支持与客户沟通反馈总结、沟通反馈中提及的材料内容（客户提供中药） 16-备注： 1）重点客户。 2）谈单承诺：赠送一份中管局标书； 3）技术路线设计的时候是两个标书，一份卫生厅标书，一份中管局标书，共用一个实验，两个标书出一份方案即可，先根据技术路线出卫生厅标书的方案，中管局标书的方案在卫生厅标书方案基础上稍作改动即可（两份标书的具体调整要求正在沟通中，会跟进反馈）； 4）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通； 5）预实验走实验项目； 6）内部留存原始数据，三次重复实验。  17-项目负责人：杨弘 </t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>N2024031302</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G70" s="14">
+        <v>45392</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>中药-有效成分-乳腺癌相关靶点的网药分析</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="14">
+        <v>45406</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号：SCI：N2024040302      国自然标书：N2024040303   02-区域-销售：王立家 03-上级主管：王立家 04-医院：浙江康复中心 05-科室： 06-电话： 07-项目（确定A/B套餐）：sci2-3分全包B套餐+国自然标书 08-分值：2-3 分 09-定题题目：SCI：养阴通脑颗粒中水蛭的关键活性成分Hirudin通过调控XX信号通路介导血管生成改善缺血性脑卒中的机制研究【方案可调整】                       国自然标书：未定题，可参考技术内容【方案可调整】              10-时间要求：SCI：2025年9月30日                        国自然标书：目前标书不急，上游未告知交付时间                    11-总价： 12-定金：已付 13-评估人员：林婧宇 14-技术支持（沟通情况）:林婧宇、薛富才（沟通次数12） 15-附件：技术路线、合同、实验报价、客户资料、技术支持与客户沟通反馈总结  16-备注： 客户要求： 1）客户分级：2.潜力客户，做项目了后续拿课题（叶总、王总同学，重要客户） 2）项目要求优先安排 ，按实验项目交付、附带作废数据。 3）网络药理学分析的时候，客户要求过来观看 4）附件技术内容是SCI 的完整内容，但是当时设计的是3-5分值的量，后来签单是2-3分，实验内容可适当删减 SCI定题可以参考技术内容定题，国自然标书就是在这个技术内容基础上挑选一部分作为预实验，并且完善研究计划，标书题目可以再大一些，再结合别的内容（免疫/代谢/微环境等） 。  内部要求： 1）内部留存原始数据，三次重复实验 2）方案在做的时候，发现技术路线和方案有较大出入的，需要跟上游和技术支持沟通【方案可调整】 17-项目负责人：杨啸 </t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>N2024040302</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>2-3 分</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G71" s="14">
+        <v>45392</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>水蛭素与缺血性脑卒中</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="14">
+        <v>45407</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">01-订单编号：IN2024042201   02-区域-销售：周燕青 03-上级主管：柳叶 04-医院：上海第九人民医院 05-科室/职称：整形外科 06-电话： 07-项目（确定A/B套餐）：生信文章（生信分析+文章写作） 08-分值：SCI 0-3分 09-定题题目：/ 10-时间要求：生信分析：2024年5月15日                       文章写作：（2024年5月16日-2024年7月16日） 11-总价： 12-定金：已付 13-评估人员 ：薛富才 14-技术支持（沟通情况）：孙慧、黄礼闯、薛富才 15-附件：合同、客户国自然面上立项依据、2023年生信服务交付内容。评估截图（关联单号： IN2023072803  2024/2/6发起过评估，慧慧知道） 16-备注： 1）客户分级：潜力客户，做项目为了后续拿课题。 2）-客户的 RNA-seq 数据集，以 DEGs 建立 PPI 网络，试分析 HNRNPH1 的作用，以及 wnt 通路。  -scRNA-seq (可能需要两组数据，瘢痕增生 (SH) 和正常组织), HNRNPH1 的作用，免疫细  胞的行为，免疫细胞的 DEGs。 -拟时分析，HNRNPH1、TCF4 的拟时表达变化等 -细胞通讯，巨噬细胞等的通讯，Wnt 通路相关基因的表达和通讯 3）姜黄素对 HNRNPH1 的作用 (直接作用还是间接，是否可以结合，可以尝试分子对接，或者从转录因子角度出发) 4）视结果整理，可做一些新的分析，或探究一些新的方法。 5）目前生信计划是根据上次沟通的几个方案都会尝试分析，抱着发文章的目的去产出不偏离课题的数据来写文章。 6）发文章目的产生的其它数据挖掘不再另外收取费用。 7）最后整理成完整分析报告（形式为本 pdf 文档），并附含上述分析的图表信息，参考文献等。生信服务交付同时需交付源代码。 8）生信分析满足技术层面输出具备sci0-3分文章写作服务、包含3次修回/2次文章修改（不包含投稿），用作客户面上课题结题。 9）以上1-8为合同中明确显示的服务内容，后续文章写作请尽量按照3分以上的标准去写作，这样客户后期自己投稿时，也可以往3分左右去投稿，尽量能在在6月中能交付初稿 17-项目负责人：杨弘 </t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>IN2024042201</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>SCI 0-3分</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G72" s="14">
+        <v>45404</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>HNRNPH1 与瘢痕增生的关联性挖掘</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4019,7 +4434,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="13">
+      <c r="A2" s="14">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -4045,7 +4460,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="14">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -4065,7 +4480,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -4091,7 +4506,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="14">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -4111,7 +4526,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -4137,7 +4552,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="14">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>

<commit_message>
Mon Jul  1 09:30:57 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary/生信组表格登记-黄礼闯.xlsx
+++ b/lixiao/summary/生信组表格登记-黄礼闯.xlsx
@@ -698,12 +698,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1053,7 +1055,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1099,7 +1101,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>45106</v>
       </c>
       <c r="B2">
@@ -1125,7 +1127,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="5">
         <v>45102</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -1145,7 +1147,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>45114</v>
       </c>
       <c r="B3">
@@ -1171,7 +1173,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="5">
         <v>45110</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -1191,7 +1193,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>45156</v>
       </c>
       <c r="B4">
@@ -1217,7 +1219,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>45145</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -1237,7 +1239,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>45190</v>
       </c>
       <c r="B5">
@@ -1263,7 +1265,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="5">
         <v>45162</v>
       </c>
       <c r="H5" t="inlineStr">
@@ -1283,7 +1285,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <v>45177</v>
       </c>
       <c r="B6">
@@ -1309,7 +1311,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="5">
         <v>45155</v>
       </c>
       <c r="H6" t="inlineStr">
@@ -1329,7 +1331,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="5">
         <v>45190</v>
       </c>
       <c r="B7">
@@ -1355,7 +1357,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="5">
         <v>45162</v>
       </c>
       <c r="H7" t="inlineStr">
@@ -1375,7 +1377,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>45197</v>
       </c>
       <c r="B8">
@@ -1401,7 +1403,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="5">
         <v>45181</v>
       </c>
       <c r="H8" t="inlineStr">
@@ -1421,7 +1423,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>45188</v>
       </c>
       <c r="B9">
@@ -1447,7 +1449,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="5">
         <v>45181</v>
       </c>
       <c r="H9" t="inlineStr">
@@ -1467,7 +1469,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>45208</v>
       </c>
       <c r="B10">
@@ -1493,7 +1495,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="5">
         <v>45204</v>
       </c>
       <c r="H10" t="inlineStr">
@@ -1513,7 +1515,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <v>45208</v>
       </c>
       <c r="B11">
@@ -1539,7 +1541,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="5">
         <v>45204</v>
       </c>
       <c r="H11" t="inlineStr">
@@ -1559,7 +1561,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3">
+      <c r="A12" s="5">
         <v>45208</v>
       </c>
       <c r="B12">
@@ -1585,7 +1587,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="5">
         <v>45204</v>
       </c>
       <c r="H12" t="inlineStr">
@@ -1605,8 +1607,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3">
-        <v>45216</v>
+      <c r="A13" s="5">
+        <v>45467</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1631,7 +1633,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="5">
         <v>45208</v>
       </c>
       <c r="H13" t="inlineStr">
@@ -1651,7 +1653,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3">
+      <c r="A14" s="5">
         <v>45219</v>
       </c>
       <c r="B14">
@@ -1677,7 +1679,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="5">
         <v>45217</v>
       </c>
       <c r="H14" t="inlineStr">
@@ -1697,7 +1699,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>45236</v>
       </c>
       <c r="B15">
@@ -1723,7 +1725,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="5">
         <v>45236</v>
       </c>
       <c r="H15" t="inlineStr">
@@ -1743,7 +1745,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3">
+      <c r="A16" s="5">
         <v>45240</v>
       </c>
       <c r="B16">
@@ -1769,7 +1771,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="5">
         <v>45237</v>
       </c>
       <c r="H16" t="inlineStr">
@@ -1789,7 +1791,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3">
+      <c r="A17" s="5">
         <v>45258</v>
       </c>
       <c r="B17">
@@ -1815,7 +1817,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="5">
         <v>45244</v>
       </c>
       <c r="H17" t="inlineStr">
@@ -1835,7 +1837,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3">
+      <c r="A18" s="5">
         <v>45247</v>
       </c>
       <c r="B18">
@@ -1861,7 +1863,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="5">
         <v>45245</v>
       </c>
       <c r="H18" t="inlineStr">
@@ -1881,7 +1883,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3">
+      <c r="A19" s="5">
         <v>45252</v>
       </c>
       <c r="B19">
@@ -1907,7 +1909,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="5">
         <v>45246</v>
       </c>
       <c r="H19" t="inlineStr">
@@ -1927,7 +1929,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3">
+      <c r="A20" s="5">
         <v>45257</v>
       </c>
       <c r="B20">
@@ -1953,7 +1955,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="5">
         <v>45253</v>
       </c>
       <c r="H20" t="inlineStr">
@@ -1973,7 +1975,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3">
+      <c r="A21" s="5">
         <v>45264</v>
       </c>
       <c r="B21">
@@ -1999,7 +2001,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="5">
         <v>45260</v>
       </c>
       <c r="H21" t="inlineStr">
@@ -2019,7 +2021,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3">
+      <c r="A22" s="5">
         <v>45265</v>
       </c>
       <c r="B22">
@@ -2045,7 +2047,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="5">
         <v>45264</v>
       </c>
       <c r="H22" t="inlineStr">
@@ -2065,7 +2067,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3">
+      <c r="A23" s="5">
         <v>45272</v>
       </c>
       <c r="B23">
@@ -2091,7 +2093,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="5">
         <v>45264</v>
       </c>
       <c r="H23" t="inlineStr">
@@ -2111,7 +2113,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3">
+      <c r="A24" s="5">
         <v>45266</v>
       </c>
       <c r="B24">
@@ -2137,7 +2139,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="5">
         <v>45266</v>
       </c>
       <c r="H24" t="inlineStr">
@@ -2157,7 +2159,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3">
+      <c r="A25" s="5">
         <v>45266</v>
       </c>
       <c r="B25">
@@ -2183,7 +2185,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="5">
         <v>45266</v>
       </c>
       <c r="H25" t="inlineStr">
@@ -2203,7 +2205,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3">
+      <c r="A26" s="5">
         <v>45268</v>
       </c>
       <c r="B26">
@@ -2229,7 +2231,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="5">
         <v>45267</v>
       </c>
       <c r="H26" t="inlineStr">
@@ -2249,7 +2251,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3">
+      <c r="A27" s="5">
         <v>45275</v>
       </c>
       <c r="B27">
@@ -2275,7 +2277,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="5">
         <v>45272</v>
       </c>
       <c r="H27" t="inlineStr">
@@ -2295,7 +2297,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3">
+      <c r="A28" s="5">
         <v>45273</v>
       </c>
       <c r="B28">
@@ -2321,7 +2323,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="5">
         <v>45272</v>
       </c>
       <c r="H28" t="inlineStr">
@@ -2341,7 +2343,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3">
+      <c r="A29" s="5">
         <v>45274</v>
       </c>
       <c r="B29">
@@ -2367,7 +2369,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="5">
         <v>45274</v>
       </c>
       <c r="H29" t="inlineStr">
@@ -2387,7 +2389,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3">
+      <c r="A30" s="5">
         <v>45359</v>
       </c>
       <c r="B30">
@@ -2413,7 +2415,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="5">
         <v>45274</v>
       </c>
       <c r="H30" t="inlineStr">
@@ -2433,7 +2435,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3">
+      <c r="A31" s="5">
         <v>45293</v>
       </c>
       <c r="B31">
@@ -2459,7 +2461,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="5">
         <v>45281</v>
       </c>
       <c r="H31" t="inlineStr">
@@ -2479,7 +2481,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3">
+      <c r="A32" s="5">
         <v>45285</v>
       </c>
       <c r="B32">
@@ -2505,7 +2507,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="5">
         <v>45281</v>
       </c>
       <c r="H32" t="inlineStr">
@@ -2525,7 +2527,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3">
+      <c r="A33" s="5">
         <v>45306</v>
       </c>
       <c r="B33">
@@ -2551,7 +2553,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="5">
         <v>45288</v>
       </c>
       <c r="H33" t="inlineStr">
@@ -2571,7 +2573,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3">
+      <c r="A34" s="5">
         <v>45363</v>
       </c>
       <c r="B34">
@@ -2597,7 +2599,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="5">
         <v>45299</v>
       </c>
       <c r="H34" t="inlineStr">
@@ -2617,7 +2619,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3">
+      <c r="A35" s="5">
         <v>45322</v>
       </c>
       <c r="B35">
@@ -2643,7 +2645,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="5">
         <v>45299</v>
       </c>
       <c r="H35" t="inlineStr">
@@ -2663,7 +2665,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3">
+      <c r="A36" s="5">
         <v>45323</v>
       </c>
       <c r="B36">
@@ -2689,7 +2691,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="5">
         <v>45302</v>
       </c>
       <c r="H36" t="inlineStr">
@@ -2709,7 +2711,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="3">
+      <c r="A37" s="5">
         <v>45322</v>
       </c>
       <c r="B37">
@@ -2735,7 +2737,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="5">
         <v>45303</v>
       </c>
       <c r="H37" t="inlineStr">
@@ -2755,7 +2757,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="3">
+      <c r="A38" s="5">
         <v>45322</v>
       </c>
       <c r="B38">
@@ -2781,7 +2783,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="5">
         <v>45314</v>
       </c>
       <c r="H38" t="inlineStr">
@@ -2801,8 +2803,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3">
-        <v>45439</v>
+      <c r="A39" s="5">
+        <v>45446</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -2827,7 +2829,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="5">
         <v>45317</v>
       </c>
       <c r="H39" t="inlineStr">
@@ -2842,12 +2844,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 基因注释、信息获取; (2) KEGG、GO富集分析; (3) fastq 文件预处理、对齐参考基因; (4) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (5) 获取疾病或条件相关的基因集:Genecards; (6) limma, edgeR 差异分析; (7) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等; (8) 宏基因组数据分析</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3">
+      <c r="A40" s="5">
         <v>45363</v>
       </c>
       <c r="B40">
@@ -2873,7 +2875,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="5">
         <v>45299</v>
       </c>
       <c r="H40" t="inlineStr">
@@ -2893,7 +2895,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3">
+      <c r="A41" s="5">
         <v>45322</v>
       </c>
       <c r="B41">
@@ -2919,7 +2921,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="5">
         <v>45300</v>
       </c>
       <c r="H41" t="inlineStr">
@@ -2939,7 +2941,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="3">
+      <c r="A42" s="5">
         <v>45350</v>
       </c>
       <c r="B42">
@@ -2965,7 +2967,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="5">
         <v>45322</v>
       </c>
       <c r="H42" t="inlineStr">
@@ -2985,7 +2987,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3">
+      <c r="A43" s="5">
         <v>45350</v>
       </c>
       <c r="B43">
@@ -3011,7 +3013,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="5">
         <v>45324</v>
       </c>
       <c r="H43" t="inlineStr">
@@ -3031,7 +3033,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3">
+      <c r="A44" s="5">
         <v>45350</v>
       </c>
       <c r="B44">
@@ -3057,7 +3059,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="5">
         <v>45324</v>
       </c>
       <c r="H44" t="inlineStr">
@@ -3077,7 +3079,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3">
+      <c r="A45" s="5">
         <v>45350</v>
       </c>
       <c r="B45">
@@ -3103,7 +3105,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="5">
         <v>45326</v>
       </c>
       <c r="H45" t="inlineStr">
@@ -3123,7 +3125,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="3">
+      <c r="A46" s="5">
         <v>45351</v>
       </c>
       <c r="B46">
@@ -3149,7 +3151,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="5">
         <v>45343</v>
       </c>
       <c r="H46" t="inlineStr">
@@ -3169,7 +3171,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3">
+      <c r="A47" s="5">
         <v>45352</v>
       </c>
       <c r="B47">
@@ -3195,7 +3197,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="5">
         <v>45344</v>
       </c>
       <c r="H47" t="inlineStr">
@@ -3215,7 +3217,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="3">
+      <c r="A48" s="5">
         <v>45351</v>
       </c>
       <c r="B48">
@@ -3241,7 +3243,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="5">
         <v>45345</v>
       </c>
       <c r="H48" t="inlineStr">
@@ -3261,7 +3263,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="3">
+      <c r="A49" s="5">
         <v>45351</v>
       </c>
       <c r="B49">
@@ -3287,7 +3289,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="5">
         <v>45351</v>
       </c>
       <c r="H49" t="inlineStr">
@@ -3307,7 +3309,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="3">
+      <c r="A50" s="5">
         <v>45351</v>
       </c>
       <c r="B50">
@@ -3333,7 +3335,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="5">
         <v>45351</v>
       </c>
       <c r="H50" t="inlineStr">
@@ -3353,7 +3355,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3">
+      <c r="A51" s="5">
         <v>45351</v>
       </c>
       <c r="B51">
@@ -3379,7 +3381,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="5">
         <v>45351</v>
       </c>
       <c r="H51" t="inlineStr">
@@ -3399,7 +3401,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="3">
+      <c r="A52" s="5">
         <v>45406</v>
       </c>
       <c r="B52">
@@ -3425,7 +3427,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="5">
         <v>45344</v>
       </c>
       <c r="H52" t="inlineStr">
@@ -3445,7 +3447,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="3">
+      <c r="A53" s="5">
         <v>45355</v>
       </c>
       <c r="B53">
@@ -3471,7 +3473,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="5">
         <v>45345</v>
       </c>
       <c r="H53" t="inlineStr">
@@ -3491,7 +3493,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="3">
+      <c r="A54" s="5">
         <v>45363</v>
       </c>
       <c r="B54">
@@ -3517,7 +3519,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="5">
         <v>45351</v>
       </c>
       <c r="H54" t="inlineStr">
@@ -3537,7 +3539,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="3">
+      <c r="A55" s="5">
         <v>45356</v>
       </c>
       <c r="B55">
@@ -3563,7 +3565,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="5">
         <v>45355</v>
       </c>
       <c r="H55" t="inlineStr">
@@ -3583,7 +3585,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="3">
+      <c r="A56" s="5">
         <v>45369</v>
       </c>
       <c r="B56">
@@ -3609,7 +3611,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="5">
         <v>45355</v>
       </c>
       <c r="H56" t="inlineStr">
@@ -3629,7 +3631,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="3">
+      <c r="A57" s="5">
         <v>45357</v>
       </c>
       <c r="B57">
@@ -3655,7 +3657,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="5">
         <v>45356</v>
       </c>
       <c r="H57" t="inlineStr">
@@ -3675,7 +3677,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="3">
+      <c r="A58" s="5">
         <v>45378</v>
       </c>
       <c r="B58">
@@ -3701,7 +3703,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="5">
         <v>45359</v>
       </c>
       <c r="H58" t="inlineStr">
@@ -3721,7 +3723,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="3">
+      <c r="A59" s="5">
         <v>45366</v>
       </c>
       <c r="B59">
@@ -3747,7 +3749,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="5">
         <v>45364</v>
       </c>
       <c r="H59" t="inlineStr">
@@ -3767,7 +3769,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="3">
+      <c r="A60" s="5">
         <v>45379</v>
       </c>
       <c r="B60">
@@ -3793,7 +3795,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="5">
         <v>45370</v>
       </c>
       <c r="H60" t="inlineStr">
@@ -3813,7 +3815,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="3">
+      <c r="A61" s="5">
         <v>45376</v>
       </c>
       <c r="B61">
@@ -3839,7 +3841,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="5">
         <v>45374</v>
       </c>
       <c r="H61" t="inlineStr">
@@ -3859,7 +3861,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="3">
+      <c r="A62" s="5">
         <v>45379</v>
       </c>
       <c r="B62">
@@ -3885,7 +3887,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="5">
         <v>45379</v>
       </c>
       <c r="H62" t="inlineStr">
@@ -3905,7 +3907,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="3">
+      <c r="A63" s="5">
         <v>45406</v>
       </c>
       <c r="B63">
@@ -3931,7 +3933,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="5">
         <v>45344</v>
       </c>
       <c r="H63" t="inlineStr">
@@ -3951,7 +3953,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="3">
+      <c r="A64" s="5">
         <v>45401</v>
       </c>
       <c r="B64">
@@ -3977,7 +3979,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="5">
         <v>45378</v>
       </c>
       <c r="H64" t="inlineStr">
@@ -3997,8 +3999,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="3">
-        <v>45435</v>
+      <c r="A65" s="5">
+        <v>45446</v>
       </c>
       <c r="B65">
         <v>64</v>
@@ -4023,7 +4025,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="5">
         <v>45384</v>
       </c>
       <c r="H65" t="inlineStr">
@@ -4038,12 +4040,12 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) KEGG、GO富集分析; (2) 表观遗传调控因子数据获取; (3) 获取疾病或条件相关的基因集:Genecards; (4) limma, edgeR 差异分析; (5) 药物临床化疗反应预测、耐药性预测; (6) 构建 PPI 网络; (7) TCGA 数据挖掘和常规分析</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="3">
+      <c r="A66" s="5">
         <v>45407</v>
       </c>
       <c r="B66">
@@ -4069,7 +4071,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="5">
         <v>45384</v>
       </c>
       <c r="H66" t="inlineStr">
@@ -4089,8 +4091,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="3">
-        <v>45418</v>
+      <c r="A67" s="5">
+        <v>45446</v>
       </c>
       <c r="B67">
         <v>66</v>
@@ -4115,7 +4117,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G67" s="3">
+      <c r="G67" s="5">
         <v>45385</v>
       </c>
       <c r="H67" t="inlineStr">
@@ -4130,12 +4132,12 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 基因注释、信息获取; (2) 获取疾病或条件相关的基因集:Genecards; (3) 从 GEO 挖掘可用数据:RNA-seq; (4) limma, edgeR 差异分析; (5) 单细胞数据分析注释细胞群</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="3">
+      <c r="A68" s="5">
         <v>45399</v>
       </c>
       <c r="B68">
@@ -4161,7 +4163,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G68" s="3">
+      <c r="G68" s="5">
         <v>45389</v>
       </c>
       <c r="H68" t="inlineStr">
@@ -4181,7 +4183,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="3">
+      <c r="A69" s="5">
         <v>45392</v>
       </c>
       <c r="B69">
@@ -4207,7 +4209,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G69" s="3">
+      <c r="G69" s="5">
         <v>45391</v>
       </c>
       <c r="H69" t="inlineStr">
@@ -4227,8 +4229,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="3">
-        <v>45434</v>
+      <c r="A70" s="5">
+        <v>45446</v>
       </c>
       <c r="B70">
         <v>69</v>
@@ -4253,7 +4255,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G70" s="3">
+      <c r="G70" s="5">
         <v>45392</v>
       </c>
       <c r="H70" t="inlineStr">
@@ -4268,12 +4270,12 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) KEGG、GO富集分析; (2) 获取疾病或条件相关的基因集:Genecards; (3) limma, edgeR 差异分析; (4) TCMSP 数据库数据挖掘; (5) 网络药理学; (6) 蛋白质信息获取</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="3">
+      <c r="A71" s="5">
         <v>45406</v>
       </c>
       <c r="B71">
@@ -4299,7 +4301,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G71" s="3">
+      <c r="G71" s="5">
         <v>45392</v>
       </c>
       <c r="H71" t="inlineStr">
@@ -4319,8 +4321,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="3">
-        <v>45439</v>
+      <c r="A72" s="5">
+        <v>45446</v>
       </c>
       <c r="B72">
         <v>71</v>
@@ -4345,7 +4347,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G72" s="3">
+      <c r="G72" s="5">
         <v>45317</v>
       </c>
       <c r="H72" t="inlineStr">
@@ -4360,12 +4362,12 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 基因注释、信息获取; (2) KEGG、GO富集分析; (3) fastq 文件预处理、对齐参考基因; (4) 肠道菌数据和代谢物数据联合分析:通过公共数据挖掘建立联系; (5) 获取疾病或条件相关的基因集:Genecards; (6) limma, edgeR 差异分析; (7) 常规 16s RNA 肠道菌数据分析:alpha多样性+beta多样性+biomarker筛选等; (8) 宏基因组数据分析</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="3">
+      <c r="A73" s="5">
         <v>45443</v>
       </c>
       <c r="B73">
@@ -4391,7 +4393,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G73" s="3">
+      <c r="G73" s="5">
         <v>45383</v>
       </c>
       <c r="H73" t="inlineStr">
@@ -4406,13 +4408,13 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 基因注释、信息获取; (2) 差异甲基化分析、可视化; (3) KEGG、GO富集分析; (4) 多数据库获取疾病靶点; (5) limma, edgeR 差异分析; (6) 构建 PPI 网络; (7) UCSC table 数据获取、基因位点注释; (8) CpG islands 数据获取</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="3">
-        <v>45435</v>
+      <c r="A74" s="5">
+        <v>45446</v>
       </c>
       <c r="B74">
         <v>73</v>
@@ -4437,7 +4439,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G74" s="3">
+      <c r="G74" s="5">
         <v>45384</v>
       </c>
       <c r="H74" t="inlineStr">
@@ -4452,13 +4454,13 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) KEGG、GO富集分析; (2) 表观遗传调控因子数据获取; (3) 获取疾病或条件相关的基因集:Genecards; (4) limma, edgeR 差异分析; (5) 药物临床化疗反应预测、耐药性预测; (6) 构建 PPI 网络; (7) TCGA 数据挖掘和常规分析</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="3">
-        <v>45418</v>
+      <c r="A75" s="5">
+        <v>45446</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -4483,7 +4485,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G75" s="3">
+      <c r="G75" s="5">
         <v>45385</v>
       </c>
       <c r="H75" t="inlineStr">
@@ -4498,13 +4500,13 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 基因注释、信息获取; (2) 获取疾病或条件相关的基因集:Genecards; (3) 从 GEO 挖掘可用数据:RNA-seq; (4) limma, edgeR 差异分析; (5) 单细胞数据分析注释细胞群</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="3">
-        <v>45434</v>
+      <c r="A76" s="5">
+        <v>45446</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -4529,7 +4531,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G76" s="3">
+      <c r="G76" s="5">
         <v>45392</v>
       </c>
       <c r="H76" t="inlineStr">
@@ -4544,13 +4546,13 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) KEGG、GO富集分析; (2) 获取疾病或条件相关的基因集:Genecards; (3) limma, edgeR 差异分析; (4) TCMSP 数据库数据挖掘; (5) 网络药理学; (6) 蛋白质信息获取</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="3">
-        <v>45425</v>
+      <c r="A77" s="5">
+        <v>45463</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -4575,7 +4577,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G77" s="3">
+      <c r="G77" s="5">
         <v>45404</v>
       </c>
       <c r="H77" t="inlineStr">
@@ -4590,13 +4592,13 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t/>
+          <t>(1) 单细胞细胞通讯; (2) 构建 PPI 网络; (3) KEGG、GO富集分析; (4) GSEA 富集分析; (5) 从 GEO 挖掘可用数据:RNA-seq; (6) limma, edgeR 差异分析; (7) 单细胞拟时分析; (8) 单细胞数据分析注释细胞群; (9) 全自动批量分子对接</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="3">
-        <v>45439</v>
+      <c r="A78" s="5">
+        <v>45446</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -4621,7 +4623,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G78" s="3">
+      <c r="G78" s="5">
         <v>45422</v>
       </c>
       <c r="H78" t="inlineStr">
@@ -4635,6 +4637,190 @@
         </is>
       </c>
       <c r="J78" t="inlineStr">
+        <is>
+          <t>(1) 基因注释、信息获取; (2) 单细胞数据预测代谢通量; (3) KEGG、GO富集分析; (4) 从 GEO 挖掘可用数据:RNA-seq; (5) 获取疾病或条件相关的基因集:Genecards; (6) limma, edgeR 差异分析; (7) 单细胞拟时分析; (8) 构建 PPI 网络; (9) 单细胞数据分析注释细胞群; (10) 调控该基因的相关转录因子 (TF) 数据获取</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5">
+        <v>45470</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G79" s="5">
+        <v>45191</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>图片查重程序</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="5">
+        <v>45462</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>曹卓订单</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G80" s="5">
+        <v>45462</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>空代+空转+单细胞的联合分析</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5">
+        <v>45467</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>筛选研究对象AA菌-BB代谢产物-XX基因</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G81" s="5">
+        <v>45464</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>筛选研究对象AA菌-BB代谢产物-XX基因</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>(1) 基因注释、信息获取; (2) 从 GEO 挖掘可用数据:RNA-seq; (3) limma, edgeR 差异分析</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5">
+        <v>45467</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>report</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="G82" s="5">
+        <v>45467</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>报告呈现优化</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4697,7 +4883,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>45163</v>
       </c>
       <c r="B2">
@@ -4723,7 +4909,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="5">
         <v>45139</v>
       </c>
       <c r="H2" t="inlineStr">
@@ -4743,7 +4929,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>45231</v>
       </c>
       <c r="B3">
@@ -4769,7 +4955,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="5">
         <v>45196</v>
       </c>
       <c r="H3" t="inlineStr">
@@ -4789,7 +4975,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>45251</v>
       </c>
       <c r="B4">
@@ -4815,7 +5001,7 @@
           <t>黄礼闯</t>
         </is>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>45231</v>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>